<commit_message>
template fixes and natsort block removed
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2396E5BE-CCD8-49D7-98E1-2CF85A84708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC892CAA-6AA8-4C74-A878-A3933B2279F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="364">
   <si>
     <t>No</t>
   </si>
@@ -781,9 +781,6 @@
     <t>Process Planning</t>
   </si>
   <si>
-    <t>Assessment</t>
-  </si>
-  <si>
     <t>#043673</t>
   </si>
   <si>
@@ -1126,9 +1123,6 @@
     <t>[{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Fee Order: Submission of Exemption Request", "is_active": false }]</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised DPD Development (Proponent Time)","work_type_id": 65 "ea_act_id": 3, "event_name": "Start of DPD Development", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Add PHASE "Revised DPD Development (Proponent Time)" (a renamed copy of original Exemption Order PHASE),Add PHASE "Readiness Decision" from workType EAC Assessment,Add PHASE "Process Planning" from workType EAC Assessment,Add PHASE "EAC Application Development (Proponent Time)" from workType EAC Assessment,Add PHASE "EAC Application Review" from workType EAC Assessment,Add PHASE "Revised EAC Application Development (Proponent Time)" from workType EAC Assessment,Add PHASE "Effects Assessment &amp; Recommendation" from workType EAC Assessment,Add PHASE "EAC Decision" from workType EAC Assessment</t>
   </si>
   <si>
@@ -1145,18 +1139,28 @@
   </si>
   <si>
     <t>[{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Last Day of Further Readiness Decision", "start_at": 7 }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1318,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1335,14 +1339,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1351,7 +1355,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1363,13 +1367,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1378,20 +1382,20 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1400,31 +1404,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1437,7 +1441,10 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6716,10 +6723,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6985,11 +6992,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -7214,7 +7221,7 @@
         <v>242</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>11</v>
@@ -7226,7 +7233,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>23</v>
@@ -7240,10 +7247,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>11</v>
@@ -7269,10 +7276,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>11</v>
@@ -7284,7 +7291,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
@@ -7298,10 +7305,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>11</v>
@@ -7327,10 +7334,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>11</v>
@@ -7342,7 +7349,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>23</v>
@@ -7356,10 +7363,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>11</v>
@@ -7371,7 +7378,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
@@ -7969,7 +7976,7 @@
           <x14:formula1>
             <xm:f>Lookups!$B$3:$B$16</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C7</xm:sqref>
+          <xm:sqref>C2:C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
@@ -7988,7 +7995,7 @@
   <dimension ref="A1:M335"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D131" sqref="D131"/>
@@ -13280,7 +13287,7 @@
         <v>6</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E131" s="4" t="str">
         <f>IF((C131=""),"",VLOOKUP(C131,Phases!$A$2:$B$7,2,FALSE))</f>
@@ -13442,7 +13449,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E135" s="4" t="str">
         <f>IF((C135=""),"",VLOOKUP(C135,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13481,7 +13488,7 @@
         <v>7</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E136" s="4" t="str">
         <f>IF((C136=""),"",VLOOKUP(C136,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13523,7 +13530,7 @@
         <v>7</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E137" s="4" t="str">
         <f>IF((C137=""),"",VLOOKUP(C137,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13565,7 +13572,7 @@
         <v>7</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E138" s="4" t="str">
         <f>IF((C138=""),"",VLOOKUP(C138,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13604,7 +13611,7 @@
         <v>7</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E139" s="4" t="str">
         <f>IF((C139=""),"",VLOOKUP(C139,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13850,7 +13857,7 @@
         <v>7</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E145" s="4" t="str">
         <f>IF((C145=""),"",VLOOKUP(C145,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13889,7 +13896,7 @@
         <v>7</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E146" s="4" t="str">
         <f>IF((C146=""),"",VLOOKUP(C146,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13931,7 +13938,7 @@
         <v>7</v>
       </c>
       <c r="D147" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E147" s="4" t="str">
         <f>IF((C147=""),"",VLOOKUP(C147,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14009,7 +14016,7 @@
         <v>7</v>
       </c>
       <c r="D149" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E149" s="4" t="str">
         <f>IF((C149=""),"",VLOOKUP(C149,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14048,7 +14055,7 @@
         <v>7</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E150" s="4" t="str">
         <f>IF((C150=""),"",VLOOKUP(C150,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14087,7 +14094,7 @@
         <v>7</v>
       </c>
       <c r="D151" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E151" s="4" t="str">
         <f>IF((C151=""),"",VLOOKUP(C151,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14780,7 +14787,7 @@
         <v>7</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E168" s="4" t="str">
         <f>IF((C168=""),"",VLOOKUP(C168,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14822,7 +14829,7 @@
         <v>7</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E169" s="4" t="str">
         <f>IF((C169=""),"",VLOOKUP(C169,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14864,7 +14871,7 @@
         <v>7</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E170" s="4" t="str">
         <f>IF((C170=""),"",VLOOKUP(C170,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14903,7 +14910,7 @@
         <v>7</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E171" s="4" t="str">
         <f>IF((C171=""),"",VLOOKUP(C171,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14945,7 +14952,7 @@
         <v>7</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E172" s="4" t="str">
         <f>IF((C172=""),"",VLOOKUP(C172,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14987,7 +14994,7 @@
         <v>7</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E173" s="4" t="str">
         <f>IF((C173=""),"",VLOOKUP(C173,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15311,7 +15318,7 @@
         <v>7</v>
       </c>
       <c r="D181" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E181" s="4" t="str">
         <f>IF((C181=""),"",VLOOKUP(C181,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15353,7 +15360,7 @@
         <v>7</v>
       </c>
       <c r="D182" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E182" s="4" t="str">
         <f>IF((C182=""),"",VLOOKUP(C182,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15395,7 +15402,7 @@
         <v>7</v>
       </c>
       <c r="D183" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E183" s="4" t="str">
         <f>IF((C183=""),"",VLOOKUP(C183,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15434,7 +15441,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E184" s="4" t="str">
         <f>IF((C184=""),"",VLOOKUP(C184,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15473,7 +15480,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E185" s="4" t="str">
         <f>IF((C185=""),"",VLOOKUP(C185,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15515,7 +15522,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E186" s="4" t="str">
         <f>IF((C186=""),"",VLOOKUP(C186,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15593,7 +15600,7 @@
         <v>8</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E188" s="4" t="str">
         <f>IF((C188=""),"",VLOOKUP(C188,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15635,7 +15642,7 @@
         <v>8</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E189" s="4" t="str">
         <f>IF((C189=""),"",VLOOKUP(C189,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16163,7 +16170,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E202" s="4" t="str">
         <f>IF((C202=""),"",VLOOKUP(C202,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16202,7 +16209,7 @@
         <v>9</v>
       </c>
       <c r="D203" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E203" s="4" t="str">
         <f>IF((C203=""),"",VLOOKUP(C203,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16244,7 +16251,7 @@
         <v>9</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E204" s="4" t="str">
         <f>IF((C204=""),"",VLOOKUP(C204,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16286,7 +16293,7 @@
         <v>9</v>
       </c>
       <c r="D205" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E205" s="4" t="str">
         <f>IF((C205=""),"",VLOOKUP(C205,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16532,7 +16539,7 @@
         <v>9</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E211" s="4" t="str">
         <f>IF((C211=""),"",VLOOKUP(C211,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16574,7 +16581,7 @@
         <v>9</v>
       </c>
       <c r="D212" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E212" s="4" t="str">
         <f>IF((C212=""),"",VLOOKUP(C212,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16613,7 +16620,7 @@
         <v>9</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E213" s="4" t="str">
         <f>IF((C213=""),"",VLOOKUP(C213,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16655,7 +16662,7 @@
         <v>9</v>
       </c>
       <c r="D214" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E214" s="4" t="str">
         <f>IF((C214=""),"",VLOOKUP(C214,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16733,7 +16740,7 @@
         <v>9</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E216" s="4" t="str">
         <f>IF((C216=""),"",VLOOKUP(C216,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16775,7 +16782,7 @@
         <v>9</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E217" s="4" t="str">
         <f>IF((C217=""),"",VLOOKUP(C217,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17468,7 +17475,7 @@
         <v>9</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E234" s="4" t="str">
         <f>IF((C234=""),"",VLOOKUP(C234,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17510,7 +17517,7 @@
         <v>9</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E235" s="4" t="str">
         <f>IF((C235=""),"",VLOOKUP(C235,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17552,7 +17559,7 @@
         <v>9</v>
       </c>
       <c r="D236" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E236" s="4" t="str">
         <f>IF((C236=""),"",VLOOKUP(C236,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17591,7 +17598,7 @@
         <v>9</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E237" s="4" t="str">
         <f>IF((C237=""),"",VLOOKUP(C237,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17633,7 +17640,7 @@
         <v>9</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E238" s="4" t="str">
         <f>IF((C238=""),"",VLOOKUP(C238,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17675,7 +17682,7 @@
         <v>9</v>
       </c>
       <c r="D239" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E239" s="4" t="str">
         <f>IF((C239=""),"",VLOOKUP(C239,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17999,7 +18006,7 @@
         <v>9</v>
       </c>
       <c r="D247" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E247" s="4" t="str">
         <f>IF((C247=""),"",VLOOKUP(C247,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18041,7 +18048,7 @@
         <v>9</v>
       </c>
       <c r="D248" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E248" s="4" t="str">
         <f>IF((C248=""),"",VLOOKUP(C248,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18083,7 +18090,7 @@
         <v>9</v>
       </c>
       <c r="D249" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E249" s="4" t="str">
         <f>IF((C249=""),"",VLOOKUP(C249,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18122,7 +18129,7 @@
         <v>10</v>
       </c>
       <c r="D250" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E250" s="4" t="str">
         <f>IF((C250=""),"",VLOOKUP(C250,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18161,7 +18168,7 @@
         <v>10</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E251" s="4" t="str">
         <f>IF((C251=""),"",VLOOKUP(C251,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18200,7 +18207,7 @@
         <v>10</v>
       </c>
       <c r="D252" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E252" s="4" t="str">
         <f>IF((C252=""),"",VLOOKUP(C252,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18242,7 +18249,7 @@
         <v>10</v>
       </c>
       <c r="D253" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E253" s="4" t="str">
         <f>IF((C253=""),"",VLOOKUP(C253,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18320,7 +18327,7 @@
         <v>10</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E255" s="4" t="str">
         <f>IF((C255=""),"",VLOOKUP(C255,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18362,7 +18369,7 @@
         <v>10</v>
       </c>
       <c r="D256" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E256" s="4" t="str">
         <f>IF((C256=""),"",VLOOKUP(C256,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18890,7 +18897,7 @@
         <v>10</v>
       </c>
       <c r="D269" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E269" s="4" t="str">
         <f>IF((C269=""),"",VLOOKUP(C269,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18929,7 +18936,7 @@
         <v>10</v>
       </c>
       <c r="D270" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E270" s="4" t="str">
         <f>IF((C270=""),"",VLOOKUP(C270,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18968,7 +18975,7 @@
         <v>10</v>
       </c>
       <c r="D271" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E271" s="4" t="str">
         <f>IF((C271=""),"",VLOOKUP(C271,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19007,7 +19014,7 @@
         <v>11</v>
       </c>
       <c r="D272" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E272" s="4" t="str">
         <f>IF((C272=""),"",VLOOKUP(C272,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19049,7 +19056,7 @@
         <v>11</v>
       </c>
       <c r="D273" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E273" s="4" t="str">
         <f>IF((C273=""),"",VLOOKUP(C273,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19091,7 +19098,7 @@
         <v>11</v>
       </c>
       <c r="D274" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E274" s="4" t="str">
         <f>IF((C274=""),"",VLOOKUP(C274,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19130,7 +19137,7 @@
         <v>11</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E275" s="4" t="str">
         <f>IF((C275=""),"",VLOOKUP(C275,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19376,7 +19383,7 @@
         <v>11</v>
       </c>
       <c r="D281" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E281" s="4" t="str">
         <f>IF((C281=""),"",VLOOKUP(C281,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19418,7 +19425,7 @@
         <v>11</v>
       </c>
       <c r="D282" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E282" s="4" t="str">
         <f>IF((C282=""),"",VLOOKUP(C282,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19496,7 +19503,7 @@
         <v>11</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E284" s="4" t="str">
         <f>IF((C284=""),"",VLOOKUP(C284,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19538,7 +19545,7 @@
         <v>11</v>
       </c>
       <c r="D285" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E285" s="4" t="str">
         <f>IF((C285=""),"",VLOOKUP(C285,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20231,7 +20238,7 @@
         <v>11</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E302" s="4" t="str">
         <f>IF((C302=""),"",VLOOKUP(C302,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20273,7 +20280,7 @@
         <v>11</v>
       </c>
       <c r="D303" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E303" s="4" t="str">
         <f>IF((C303=""),"",VLOOKUP(C303,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20315,7 +20322,7 @@
         <v>11</v>
       </c>
       <c r="D304" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E304" s="4" t="str">
         <f>IF((C304=""),"",VLOOKUP(C304,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20354,7 +20361,7 @@
         <v>11</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E305" s="4" t="str">
         <f>IF((C305=""),"",VLOOKUP(C305,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20396,7 +20403,7 @@
         <v>11</v>
       </c>
       <c r="D306" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E306" s="4" t="str">
         <f>IF((C306=""),"",VLOOKUP(C306,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20438,7 +20445,7 @@
         <v>11</v>
       </c>
       <c r="D307" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E307" s="4" t="str">
         <f>IF((C307=""),"",VLOOKUP(C307,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20801,7 +20808,7 @@
         <v>11</v>
       </c>
       <c r="D316" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E316" s="4" t="str">
         <f>IF((C316=""),"",VLOOKUP(C316,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20843,7 +20850,7 @@
         <v>11</v>
       </c>
       <c r="D317" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E317" s="4" t="str">
         <f>IF((C317=""),"",VLOOKUP(C317,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20882,7 +20889,7 @@
         <v>12</v>
       </c>
       <c r="D318" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E318" s="4" t="str">
         <f>IF((C318=""),"",VLOOKUP(C318,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20960,7 +20967,7 @@
         <v>12</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E320" s="4" t="str">
         <f>IF((C320=""),"",VLOOKUP(C320,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21122,7 +21129,7 @@
         <v>12</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E324" s="4" t="str">
         <f>IF((C324=""),"",VLOOKUP(C324,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21164,7 +21171,7 @@
         <v>12</v>
       </c>
       <c r="D325" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E325" s="4" t="str">
         <f>IF((C325=""),"",VLOOKUP(C325,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21206,7 +21213,7 @@
         <v>12</v>
       </c>
       <c r="D326" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E326" s="4" t="str">
         <f>IF((C326=""),"",VLOOKUP(C326,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21245,7 +21252,7 @@
         <v>12</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E327" s="4" t="str">
         <f>IF((C327=""),"",VLOOKUP(C327,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21287,7 +21294,7 @@
         <v>12</v>
       </c>
       <c r="D328" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E328" s="4" t="str">
         <f>IF((C328=""),"",VLOOKUP(C328,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21329,7 +21336,7 @@
         <v>12</v>
       </c>
       <c r="D329" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E329" s="4" t="str">
         <f>IF((C329=""),"",VLOOKUP(C329,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21530,7 +21537,7 @@
         <v>12</v>
       </c>
       <c r="D334" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E334" s="4" t="str">
         <f>IF((C334=""),"",VLOOKUP(C334,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21572,7 +21579,7 @@
         <v>12</v>
       </c>
       <c r="D335" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E335" s="4" t="str">
         <f>IF((C335=""),"",VLOOKUP(C335,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -22230,7 +22237,7 @@
         <v>Federal Involvement Determination</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E31" s="2">
         <v>36</v>
@@ -22248,7 +22255,7 @@
         <v>Federal Involvement Determination</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E32" s="2">
         <v>37</v>
@@ -22266,7 +22273,7 @@
         <v>Federal Involvement Determination</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E33" s="2">
         <v>38</v>
@@ -22302,7 +22309,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E35" s="2">
         <v>40</v>
@@ -22320,7 +22327,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E36" s="2">
         <v>41</v>
@@ -22338,7 +22345,7 @@
         <v>Process Order Issued &amp; Regulatory Coordination Plan Posted</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E37" s="2">
         <v>42</v>
@@ -22410,7 +22417,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E41" s="2">
         <v>46</v>
@@ -22428,7 +22435,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E42" s="2">
         <v>47</v>
@@ -22464,7 +22471,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E44" s="2">
         <v>49</v>
@@ -22482,7 +22489,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E45" s="2">
         <v>50</v>
@@ -22500,7 +22507,7 @@
         <v>Notice to Proponent to Prepare Revised EAC Application</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E46" s="2">
         <v>51</v>
@@ -22572,7 +22579,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E50" s="2">
         <v>55</v>
@@ -22590,7 +22597,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E51" s="2">
         <v>56</v>
@@ -22608,7 +22615,7 @@
         <v>Revised EAC Application Acceptance Decision (Day Zero)</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E52" s="2">
         <v>57</v>
@@ -22626,7 +22633,7 @@
         <v>Revised EAC Application Acceptance Decision (Day Zero)</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E53" s="2">
         <v>58</v>
@@ -22662,7 +22669,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E55" s="2">
         <v>60</v>
@@ -22680,7 +22687,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E56" s="2">
         <v>61</v>
@@ -22698,7 +22705,7 @@
         <v>EAC Referral Package sent to Ministers</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E57" s="2">
         <v>62</v>
@@ -22716,7 +22723,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E58" s="2">
         <v>63</v>
@@ -22734,7 +22741,7 @@
         <v>EAC Ministers Decision</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E59" s="2">
         <v>64</v>
@@ -22752,7 +22759,7 @@
         <v>EAC Ministers Decision</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E60" s="2">
         <v>65</v>
@@ -22780,11 +22787,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -22840,7 +22847,7 @@
         <v>170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -22864,7 +22871,7 @@
         <v>170</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G3" s="2">
         <v>2</v>
@@ -22888,7 +22895,7 @@
         <v>172</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G4" s="2">
         <v>3</v>
@@ -22912,7 +22919,7 @@
         <v>174</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -22936,7 +22943,7 @@
         <v>176</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -22960,7 +22967,7 @@
         <v>178</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G7" s="2">
         <v>6</v>
@@ -22984,7 +22991,7 @@
         <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -23008,7 +23015,7 @@
         <v>181</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -23029,10 +23036,10 @@
         <v>182</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
@@ -23053,7 +23060,10 @@
         <v>183</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>362</v>
+        <v>360</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>363</v>
       </c>
       <c r="G11" s="40">
         <v>11</v>
@@ -23077,7 +23087,7 @@
         <v>185</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G12" s="2">
         <v>12</v>
@@ -23101,7 +23111,7 @@
         <v>172</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G13" s="2">
         <v>13</v>
@@ -23125,7 +23135,7 @@
         <v>174</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G14" s="2">
         <v>14</v>
@@ -23149,7 +23159,7 @@
         <v>186</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G15" s="2">
         <v>15</v>
@@ -23173,7 +23183,7 @@
         <v>178</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G16" s="2">
         <v>16</v>
@@ -23197,7 +23207,7 @@
         <v>172</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G17" s="2">
         <v>17</v>
@@ -23221,7 +23231,7 @@
         <v>174</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G18" s="2">
         <v>18</v>
@@ -23245,7 +23255,7 @@
         <v>176</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G19" s="2">
         <v>19</v>
@@ -23269,7 +23279,7 @@
         <v>178</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G20" s="2">
         <v>20</v>
@@ -23293,7 +23303,7 @@
         <v>187</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G21" s="2">
         <v>21</v>
@@ -23317,7 +23327,7 @@
         <v>170</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G22" s="2">
         <v>22</v>
@@ -23341,7 +23351,7 @@
         <v>170</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G23" s="2">
         <v>23</v>
@@ -23365,7 +23375,7 @@
         <v>172</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G24" s="2">
         <v>24</v>
@@ -23389,7 +23399,7 @@
         <v>174</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G25" s="2">
         <v>25</v>
@@ -23413,7 +23423,7 @@
         <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G26" s="2">
         <v>26</v>
@@ -23437,7 +23447,7 @@
         <v>178</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G27" s="2">
         <v>27</v>
@@ -23461,7 +23471,7 @@
         <v>172</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G28" s="2">
         <v>28</v>
@@ -23485,7 +23495,7 @@
         <v>174</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G29" s="2">
         <v>29</v>
@@ -23509,7 +23519,7 @@
         <v>176</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G30" s="2">
         <v>30</v>
@@ -23533,7 +23543,7 @@
         <v>178</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G31" s="2">
         <v>31</v>
@@ -23557,7 +23567,7 @@
         <v>188</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G32" s="2">
         <v>32</v>
@@ -23578,10 +23588,10 @@
         <v>189</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="G33" s="2">
         <v>33</v>
@@ -23605,7 +23615,7 @@
         <v>192</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G34" s="2">
         <v>36</v>
@@ -23629,7 +23639,7 @@
         <v>193</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G35" s="2">
         <v>37</v>
@@ -23653,7 +23663,7 @@
         <v>170</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G36" s="2">
         <v>38</v>
@@ -23677,7 +23687,7 @@
         <v>185</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G37" s="2">
         <v>39</v>
@@ -23701,7 +23711,7 @@
         <v>172</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G38" s="2">
         <v>40</v>
@@ -23725,7 +23735,7 @@
         <v>174</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G39" s="2">
         <v>41</v>
@@ -23749,7 +23759,7 @@
         <v>186</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G40" s="2">
         <v>42</v>
@@ -23773,7 +23783,7 @@
         <v>178</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G41" s="2">
         <v>43</v>
@@ -23797,7 +23807,7 @@
         <v>172</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G42" s="2">
         <v>44</v>
@@ -23821,7 +23831,7 @@
         <v>174</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G43" s="2">
         <v>45</v>
@@ -23845,7 +23855,7 @@
         <v>176</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G44" s="2">
         <v>46</v>
@@ -23869,7 +23879,7 @@
         <v>178</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G45" s="2">
         <v>47</v>
@@ -23893,7 +23903,7 @@
         <v>194</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G46" s="2">
         <v>48</v>
@@ -23917,7 +23927,7 @@
         <v>172</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G47" s="2">
         <v>49</v>
@@ -23941,7 +23951,7 @@
         <v>174</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G48" s="2">
         <v>50</v>
@@ -23965,7 +23975,7 @@
         <v>176</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G49" s="2">
         <v>51</v>
@@ -23989,7 +23999,7 @@
         <v>178</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G50" s="2">
         <v>52</v>
@@ -24013,7 +24023,7 @@
         <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G51" s="2">
         <v>53</v>
@@ -24037,7 +24047,7 @@
         <v>197</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G52" s="2">
         <v>54</v>
@@ -24061,7 +24071,7 @@
         <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G53" s="2">
         <v>55</v>
@@ -24085,7 +24095,7 @@
         <v>199</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G54" s="2">
         <v>56</v>
@@ -24109,7 +24119,7 @@
         <v>185</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G55" s="2">
         <v>57</v>
@@ -24133,7 +24143,7 @@
         <v>172</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G56" s="2">
         <v>58</v>
@@ -24157,7 +24167,7 @@
         <v>174</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G57" s="2">
         <v>59</v>
@@ -24181,7 +24191,7 @@
         <v>186</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G58" s="2">
         <v>60</v>
@@ -24205,7 +24215,7 @@
         <v>178</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G59" s="2">
         <v>61</v>
@@ -24229,7 +24239,7 @@
         <v>172</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G60" s="2">
         <v>62</v>
@@ -24253,7 +24263,7 @@
         <v>174</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G61" s="2">
         <v>63</v>
@@ -24277,7 +24287,7 @@
         <v>176</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G62" s="2">
         <v>64</v>
@@ -24301,7 +24311,7 @@
         <v>178</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G63" s="2">
         <v>65</v>
@@ -24322,10 +24332,10 @@
         <v>189</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F64" s="30" t="s">
         <v>351</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>352</v>
       </c>
       <c r="G64" s="2">
         <v>66</v>
@@ -24348,8 +24358,8 @@
       <c r="E65" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F65" s="30" t="s">
-        <v>358</v>
+      <c r="F65" s="43" t="s">
+        <v>352</v>
       </c>
       <c r="G65" s="2">
         <v>69</v>
@@ -24370,10 +24380,10 @@
         <v>189</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G66" s="2">
         <v>70</v>
@@ -24397,7 +24407,7 @@
         <v>190</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G67" s="2">
         <v>78</v>
@@ -24421,7 +24431,7 @@
         <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G68" s="2">
         <v>79</v>
@@ -24445,7 +24455,7 @@
         <v>201</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G69" s="38">
         <v>80</v>
@@ -24469,7 +24479,7 @@
         <v>200</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G70" s="2">
         <v>82</v>
@@ -24493,7 +24503,7 @@
         <v>202</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G71" s="2">
         <v>88</v>
@@ -24514,10 +24524,10 @@
         <v>226</v>
       </c>
       <c r="E72" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="G72" s="2">
         <v>96</v>
@@ -24538,10 +24548,10 @@
         <v>226</v>
       </c>
       <c r="E73" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="G73" s="2">
         <v>97</v>
@@ -24565,7 +24575,7 @@
         <v>202</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G74" s="2">
         <v>98</v>
@@ -24589,7 +24599,7 @@
         <v>185</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G75" s="2">
         <v>99</v>
@@ -24613,7 +24623,7 @@
         <v>172</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G76" s="2">
         <v>100</v>
@@ -24637,7 +24647,7 @@
         <v>174</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G77" s="2">
         <v>101</v>
@@ -24661,7 +24671,7 @@
         <v>186</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G78" s="2">
         <v>102</v>
@@ -24685,7 +24695,7 @@
         <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G79" s="2">
         <v>103</v>
@@ -24709,7 +24719,7 @@
         <v>172</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G80" s="2">
         <v>104</v>
@@ -24733,7 +24743,7 @@
         <v>174</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G81" s="2">
         <v>105</v>
@@ -24757,7 +24767,7 @@
         <v>176</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G82" s="2">
         <v>106</v>
@@ -24781,7 +24791,7 @@
         <v>178</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G83" s="2">
         <v>107</v>
@@ -24802,10 +24812,10 @@
         <v>191</v>
       </c>
       <c r="E84" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="F84" s="30" t="s">
         <v>331</v>
-      </c>
-      <c r="F84" s="30" t="s">
-        <v>332</v>
       </c>
       <c r="G84" s="2">
         <v>108</v>
@@ -24829,7 +24839,7 @@
         <v>170</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G85" s="2">
         <v>109</v>
@@ -24853,7 +24863,7 @@
         <v>170</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G86" s="2">
         <v>110</v>
@@ -24877,7 +24887,7 @@
         <v>185</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G87" s="2">
         <v>111</v>
@@ -24901,7 +24911,7 @@
         <v>172</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G88" s="2">
         <v>112</v>
@@ -24925,7 +24935,7 @@
         <v>174</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G89" s="2">
         <v>113</v>
@@ -24949,7 +24959,7 @@
         <v>186</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G90" s="2">
         <v>114</v>
@@ -24973,7 +24983,7 @@
         <v>178</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G91" s="2">
         <v>115</v>
@@ -24997,7 +25007,7 @@
         <v>172</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G92" s="2">
         <v>116</v>
@@ -25021,7 +25031,7 @@
         <v>174</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G93" s="2">
         <v>117</v>
@@ -25045,7 +25055,7 @@
         <v>176</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G94" s="2">
         <v>118</v>
@@ -25069,7 +25079,7 @@
         <v>178</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G95" s="2">
         <v>119</v>
@@ -25093,7 +25103,7 @@
         <v>185</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G96" s="2">
         <v>120</v>
@@ -25117,7 +25127,7 @@
         <v>172</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G97" s="2">
         <v>121</v>
@@ -25141,7 +25151,7 @@
         <v>174</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G98" s="2">
         <v>122</v>
@@ -25165,7 +25175,7 @@
         <v>186</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G99" s="2">
         <v>123</v>
@@ -25189,7 +25199,7 @@
         <v>178</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G100" s="2">
         <v>124</v>
@@ -25213,7 +25223,7 @@
         <v>172</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G101" s="2">
         <v>125</v>
@@ -25237,7 +25247,7 @@
         <v>174</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G102" s="2">
         <v>126</v>
@@ -25261,7 +25271,7 @@
         <v>176</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G103" s="2">
         <v>127</v>
@@ -25285,7 +25295,7 @@
         <v>178</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G104" s="2">
         <v>128</v>
@@ -25306,10 +25316,10 @@
         <v>191</v>
       </c>
       <c r="E105" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="F105" s="30" t="s">
         <v>333</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>334</v>
       </c>
       <c r="G105" s="2">
         <v>129</v>
@@ -25333,7 +25343,7 @@
         <v>170</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G106" s="2">
         <v>130</v>
@@ -25357,7 +25367,7 @@
         <v>170</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G107" s="2">
         <v>131</v>
@@ -25381,7 +25391,7 @@
         <v>185</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G108" s="2">
         <v>132</v>
@@ -25405,7 +25415,7 @@
         <v>172</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G109" s="2">
         <v>133</v>
@@ -25429,7 +25439,7 @@
         <v>174</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G110" s="2">
         <v>134</v>
@@ -25453,7 +25463,7 @@
         <v>186</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G111" s="2">
         <v>135</v>
@@ -25477,7 +25487,7 @@
         <v>178</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G112" s="2">
         <v>136</v>
@@ -25501,7 +25511,7 @@
         <v>172</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G113" s="2">
         <v>137</v>
@@ -25525,7 +25535,7 @@
         <v>174</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G114" s="2">
         <v>138</v>
@@ -25549,7 +25559,7 @@
         <v>176</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G115" s="2">
         <v>139</v>
@@ -25573,7 +25583,7 @@
         <v>178</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G116" s="2">
         <v>140</v>
@@ -25594,10 +25604,10 @@
         <v>191</v>
       </c>
       <c r="E117" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="F117" s="30" t="s">
         <v>335</v>
-      </c>
-      <c r="F117" s="30" t="s">
-        <v>336</v>
       </c>
       <c r="G117" s="2">
         <v>141</v>
@@ -25618,10 +25628,10 @@
         <v>182</v>
       </c>
       <c r="E118" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="G118" s="2">
         <v>142</v>
@@ -25642,10 +25652,10 @@
         <v>183</v>
       </c>
       <c r="E119" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="G119" s="2">
         <v>143</v>
@@ -25669,7 +25679,7 @@
         <v>185</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G120" s="2">
         <v>144</v>
@@ -25693,7 +25703,7 @@
         <v>172</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G121" s="2">
         <v>145</v>
@@ -25717,7 +25727,7 @@
         <v>174</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G122" s="2">
         <v>146</v>
@@ -25741,7 +25751,7 @@
         <v>186</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G123" s="2">
         <v>147</v>
@@ -25765,7 +25775,7 @@
         <v>178</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G124" s="2">
         <v>148</v>
@@ -25789,7 +25799,7 @@
         <v>172</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G125" s="2">
         <v>149</v>
@@ -25813,7 +25823,7 @@
         <v>174</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G126" s="2">
         <v>150</v>
@@ -25837,7 +25847,7 @@
         <v>176</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G127" s="2">
         <v>151</v>
@@ -25861,7 +25871,7 @@
         <v>178</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G128" s="2">
         <v>152</v>
@@ -25882,10 +25892,10 @@
         <v>191</v>
       </c>
       <c r="E129" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="F129" s="30" t="s">
         <v>341</v>
-      </c>
-      <c r="F129" s="30" t="s">
-        <v>342</v>
       </c>
       <c r="G129" s="2">
         <v>153</v>
@@ -25909,7 +25919,7 @@
         <v>172</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G130" s="2">
         <v>154</v>
@@ -25933,7 +25943,7 @@
         <v>174</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G131" s="2">
         <v>155</v>
@@ -25957,7 +25967,7 @@
         <v>176</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G132" s="2">
         <v>156</v>
@@ -25981,7 +25991,7 @@
         <v>178</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G133" s="2">
         <v>157</v>
@@ -26005,7 +26015,7 @@
         <v>195</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G134" s="2">
         <v>158</v>
@@ -26029,7 +26039,7 @@
         <v>197</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G135" s="2">
         <v>159</v>
@@ -26053,7 +26063,7 @@
         <v>195</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G136" s="2">
         <v>160</v>
@@ -26077,7 +26087,7 @@
         <v>178</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G137" s="2">
         <v>161</v>
@@ -27780,14 +27790,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28020,21 +28028,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28059,9 +28066,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
template fixes and natsort block removed (#2026)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2396E5BE-CCD8-49D7-98E1-2CF85A84708D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC892CAA-6AA8-4C74-A878-A3933B2279F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2376" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2377" uniqueCount="364">
   <si>
     <t>No</t>
   </si>
@@ -781,9 +781,6 @@
     <t>Process Planning</t>
   </si>
   <si>
-    <t>Assessment</t>
-  </si>
-  <si>
     <t>#043673</t>
   </si>
   <si>
@@ -1126,9 +1123,6 @@
     <t>[{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Fee Order: Submission of Exemption Request", "is_active": false }]</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised DPD Development (Proponent Time)","work_type_id": 65 "ea_act_id": 3, "event_name": "Start of DPD Development", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Add PHASE "Revised DPD Development (Proponent Time)" (a renamed copy of original Exemption Order PHASE),Add PHASE "Readiness Decision" from workType EAC Assessment,Add PHASE "Process Planning" from workType EAC Assessment,Add PHASE "EAC Application Development (Proponent Time)" from workType EAC Assessment,Add PHASE "EAC Application Review" from workType EAC Assessment,Add PHASE "Revised EAC Application Development (Proponent Time)" from workType EAC Assessment,Add PHASE "Effects Assessment &amp; Recommendation" from workType EAC Assessment,Add PHASE "EAC Decision" from workType EAC Assessment</t>
   </si>
   <si>
@@ -1145,18 +1139,28 @@
   </si>
   <si>
     <t>[{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Last Day of Further Readiness Decision", "start_at": 7 }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)"}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1318,7 +1322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1335,14 +1339,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1351,7 +1355,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1363,13 +1367,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1378,20 +1382,20 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1400,31 +1404,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1437,7 +1441,10 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -6716,10 +6723,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6985,11 +6992,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I158"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -7214,7 +7221,7 @@
         <v>242</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D8" s="11" t="s">
         <v>11</v>
@@ -7226,7 +7233,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="H8" s="2" t="s">
         <v>23</v>
@@ -7240,10 +7247,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D9" s="11" t="s">
         <v>11</v>
@@ -7269,10 +7276,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>11</v>
@@ -7284,7 +7291,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H10" s="2" t="s">
         <v>23</v>
@@ -7298,10 +7305,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>11</v>
@@ -7327,10 +7334,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D12" s="11" t="s">
         <v>11</v>
@@ -7342,7 +7349,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H12" s="2" t="s">
         <v>23</v>
@@ -7356,10 +7363,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D13" s="11" t="s">
         <v>11</v>
@@ -7371,7 +7378,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H13" s="2" t="s">
         <v>23</v>
@@ -7969,7 +7976,7 @@
           <x14:formula1>
             <xm:f>Lookups!$B$3:$B$16</xm:f>
           </x14:formula1>
-          <xm:sqref>C2:C7</xm:sqref>
+          <xm:sqref>C2:C13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
@@ -7988,7 +7995,7 @@
   <dimension ref="A1:M335"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="D131" sqref="D131"/>
@@ -13280,7 +13287,7 @@
         <v>6</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="E131" s="4" t="str">
         <f>IF((C131=""),"",VLOOKUP(C131,Phases!$A$2:$B$7,2,FALSE))</f>
@@ -13442,7 +13449,7 @@
         <v>7</v>
       </c>
       <c r="D135" s="18" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="E135" s="4" t="str">
         <f>IF((C135=""),"",VLOOKUP(C135,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13481,7 +13488,7 @@
         <v>7</v>
       </c>
       <c r="D136" s="29" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E136" s="4" t="str">
         <f>IF((C136=""),"",VLOOKUP(C136,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13523,7 +13530,7 @@
         <v>7</v>
       </c>
       <c r="D137" s="14" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E137" s="4" t="str">
         <f>IF((C137=""),"",VLOOKUP(C137,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13565,7 +13572,7 @@
         <v>7</v>
       </c>
       <c r="D138" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E138" s="4" t="str">
         <f>IF((C138=""),"",VLOOKUP(C138,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13604,7 +13611,7 @@
         <v>7</v>
       </c>
       <c r="D139" s="12" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E139" s="4" t="str">
         <f>IF((C139=""),"",VLOOKUP(C139,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13850,7 +13857,7 @@
         <v>7</v>
       </c>
       <c r="D145" s="12" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E145" s="4" t="str">
         <f>IF((C145=""),"",VLOOKUP(C145,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13889,7 +13896,7 @@
         <v>7</v>
       </c>
       <c r="D146" s="12" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E146" s="4" t="str">
         <f>IF((C146=""),"",VLOOKUP(C146,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -13931,7 +13938,7 @@
         <v>7</v>
       </c>
       <c r="D147" s="22" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E147" s="4" t="str">
         <f>IF((C147=""),"",VLOOKUP(C147,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14009,7 +14016,7 @@
         <v>7</v>
       </c>
       <c r="D149" s="31" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E149" s="4" t="str">
         <f>IF((C149=""),"",VLOOKUP(C149,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14048,7 +14055,7 @@
         <v>7</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E150" s="4" t="str">
         <f>IF((C150=""),"",VLOOKUP(C150,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14087,7 +14094,7 @@
         <v>7</v>
       </c>
       <c r="D151" s="31" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E151" s="4" t="str">
         <f>IF((C151=""),"",VLOOKUP(C151,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14780,7 +14787,7 @@
         <v>7</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E168" s="4" t="str">
         <f>IF((C168=""),"",VLOOKUP(C168,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14822,7 +14829,7 @@
         <v>7</v>
       </c>
       <c r="D169" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E169" s="4" t="str">
         <f>IF((C169=""),"",VLOOKUP(C169,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14864,7 +14871,7 @@
         <v>7</v>
       </c>
       <c r="D170" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E170" s="4" t="str">
         <f>IF((C170=""),"",VLOOKUP(C170,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14903,7 +14910,7 @@
         <v>7</v>
       </c>
       <c r="D171" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E171" s="4" t="str">
         <f>IF((C171=""),"",VLOOKUP(C171,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14945,7 +14952,7 @@
         <v>7</v>
       </c>
       <c r="D172" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E172" s="4" t="str">
         <f>IF((C172=""),"",VLOOKUP(C172,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -14987,7 +14994,7 @@
         <v>7</v>
       </c>
       <c r="D173" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E173" s="4" t="str">
         <f>IF((C173=""),"",VLOOKUP(C173,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15311,7 +15318,7 @@
         <v>7</v>
       </c>
       <c r="D181" s="16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E181" s="4" t="str">
         <f>IF((C181=""),"",VLOOKUP(C181,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15353,7 +15360,7 @@
         <v>7</v>
       </c>
       <c r="D182" s="32" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E182" s="4" t="str">
         <f>IF((C182=""),"",VLOOKUP(C182,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15395,7 +15402,7 @@
         <v>7</v>
       </c>
       <c r="D183" s="22" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="E183" s="4" t="str">
         <f>IF((C183=""),"",VLOOKUP(C183,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15434,7 +15441,7 @@
         <v>8</v>
       </c>
       <c r="D184" s="19" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E184" s="4" t="str">
         <f>IF((C184=""),"",VLOOKUP(C184,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15473,7 +15480,7 @@
         <v>8</v>
       </c>
       <c r="D185" s="12" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E185" s="4" t="str">
         <f>IF((C185=""),"",VLOOKUP(C185,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15515,7 +15522,7 @@
         <v>8</v>
       </c>
       <c r="D186" s="22" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="E186" s="4" t="str">
         <f>IF((C186=""),"",VLOOKUP(C186,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15593,7 +15600,7 @@
         <v>8</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E188" s="4" t="str">
         <f>IF((C188=""),"",VLOOKUP(C188,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -15635,7 +15642,7 @@
         <v>8</v>
       </c>
       <c r="D189" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E189" s="4" t="str">
         <f>IF((C189=""),"",VLOOKUP(C189,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16163,7 +16170,7 @@
         <v>8</v>
       </c>
       <c r="D202" s="16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E202" s="4" t="str">
         <f>IF((C202=""),"",VLOOKUP(C202,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16202,7 +16209,7 @@
         <v>9</v>
       </c>
       <c r="D203" s="33" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E203" s="4" t="str">
         <f>IF((C203=""),"",VLOOKUP(C203,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16244,7 +16251,7 @@
         <v>9</v>
       </c>
       <c r="D204" s="14" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E204" s="4" t="str">
         <f>IF((C204=""),"",VLOOKUP(C204,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16286,7 +16293,7 @@
         <v>9</v>
       </c>
       <c r="D205" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E205" s="4" t="str">
         <f>IF((C205=""),"",VLOOKUP(C205,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16532,7 +16539,7 @@
         <v>9</v>
       </c>
       <c r="D211" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E211" s="4" t="str">
         <f>IF((C211=""),"",VLOOKUP(C211,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16574,7 +16581,7 @@
         <v>9</v>
       </c>
       <c r="D212" s="23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E212" s="4" t="str">
         <f>IF((C212=""),"",VLOOKUP(C212,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16613,7 +16620,7 @@
         <v>9</v>
       </c>
       <c r="D213" s="1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="E213" s="4" t="str">
         <f>IF((C213=""),"",VLOOKUP(C213,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16655,7 +16662,7 @@
         <v>9</v>
       </c>
       <c r="D214" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E214" s="4" t="str">
         <f>IF((C214=""),"",VLOOKUP(C214,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16733,7 +16740,7 @@
         <v>9</v>
       </c>
       <c r="D216" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E216" s="4" t="str">
         <f>IF((C216=""),"",VLOOKUP(C216,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -16775,7 +16782,7 @@
         <v>9</v>
       </c>
       <c r="D217" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E217" s="4" t="str">
         <f>IF((C217=""),"",VLOOKUP(C217,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17468,7 +17475,7 @@
         <v>9</v>
       </c>
       <c r="D234" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E234" s="4" t="str">
         <f>IF((C234=""),"",VLOOKUP(C234,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17510,7 +17517,7 @@
         <v>9</v>
       </c>
       <c r="D235" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E235" s="4" t="str">
         <f>IF((C235=""),"",VLOOKUP(C235,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17552,7 +17559,7 @@
         <v>9</v>
       </c>
       <c r="D236" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E236" s="4" t="str">
         <f>IF((C236=""),"",VLOOKUP(C236,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17591,7 +17598,7 @@
         <v>9</v>
       </c>
       <c r="D237" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E237" s="4" t="str">
         <f>IF((C237=""),"",VLOOKUP(C237,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17633,7 +17640,7 @@
         <v>9</v>
       </c>
       <c r="D238" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E238" s="4" t="str">
         <f>IF((C238=""),"",VLOOKUP(C238,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17675,7 +17682,7 @@
         <v>9</v>
       </c>
       <c r="D239" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E239" s="4" t="str">
         <f>IF((C239=""),"",VLOOKUP(C239,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -17999,7 +18006,7 @@
         <v>9</v>
       </c>
       <c r="D247" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E247" s="4" t="str">
         <f>IF((C247=""),"",VLOOKUP(C247,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18041,7 +18048,7 @@
         <v>9</v>
       </c>
       <c r="D248" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="E248" s="4" t="str">
         <f>IF((C248=""),"",VLOOKUP(C248,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18083,7 +18090,7 @@
         <v>9</v>
       </c>
       <c r="D249" s="20" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E249" s="4" t="str">
         <f>IF((C249=""),"",VLOOKUP(C249,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18122,7 +18129,7 @@
         <v>10</v>
       </c>
       <c r="D250" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="E250" s="4" t="str">
         <f>IF((C250=""),"",VLOOKUP(C250,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18161,7 +18168,7 @@
         <v>10</v>
       </c>
       <c r="D251" s="12" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E251" s="4" t="str">
         <f>IF((C251=""),"",VLOOKUP(C251,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18200,7 +18207,7 @@
         <v>10</v>
       </c>
       <c r="D252" s="12" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E252" s="4" t="str">
         <f>IF((C252=""),"",VLOOKUP(C252,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18242,7 +18249,7 @@
         <v>10</v>
       </c>
       <c r="D253" s="22" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E253" s="4" t="str">
         <f>IF((C253=""),"",VLOOKUP(C253,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18320,7 +18327,7 @@
         <v>10</v>
       </c>
       <c r="D255" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E255" s="4" t="str">
         <f>IF((C255=""),"",VLOOKUP(C255,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18362,7 +18369,7 @@
         <v>10</v>
       </c>
       <c r="D256" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E256" s="4" t="str">
         <f>IF((C256=""),"",VLOOKUP(C256,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18890,7 +18897,7 @@
         <v>10</v>
       </c>
       <c r="D269" s="16" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E269" s="4" t="str">
         <f>IF((C269=""),"",VLOOKUP(C269,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18929,7 +18936,7 @@
         <v>10</v>
       </c>
       <c r="D270" s="14" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E270" s="4" t="str">
         <f>IF((C270=""),"",VLOOKUP(C270,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -18968,7 +18975,7 @@
         <v>10</v>
       </c>
       <c r="D271" s="20" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E271" s="4" t="str">
         <f>IF((C271=""),"",VLOOKUP(C271,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19007,7 +19014,7 @@
         <v>11</v>
       </c>
       <c r="D272" s="18" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E272" s="4" t="str">
         <f>IF((C272=""),"",VLOOKUP(C272,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19049,7 +19056,7 @@
         <v>11</v>
       </c>
       <c r="D273" s="14" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E273" s="4" t="str">
         <f>IF((C273=""),"",VLOOKUP(C273,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19091,7 +19098,7 @@
         <v>11</v>
       </c>
       <c r="D274" s="20" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E274" s="4" t="str">
         <f>IF((C274=""),"",VLOOKUP(C274,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19130,7 +19137,7 @@
         <v>11</v>
       </c>
       <c r="D275" s="1" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="E275" s="4" t="str">
         <f>IF((C275=""),"",VLOOKUP(C275,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19376,7 +19383,7 @@
         <v>11</v>
       </c>
       <c r="D281" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E281" s="4" t="str">
         <f>IF((C281=""),"",VLOOKUP(C281,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19418,7 +19425,7 @@
         <v>11</v>
       </c>
       <c r="D282" s="22" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E282" s="4" t="str">
         <f>IF((C282=""),"",VLOOKUP(C282,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19496,7 +19503,7 @@
         <v>11</v>
       </c>
       <c r="D284" s="1" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E284" s="4" t="str">
         <f>IF((C284=""),"",VLOOKUP(C284,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -19538,7 +19545,7 @@
         <v>11</v>
       </c>
       <c r="D285" s="14" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E285" s="4" t="str">
         <f>IF((C285=""),"",VLOOKUP(C285,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20231,7 +20238,7 @@
         <v>11</v>
       </c>
       <c r="D302" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E302" s="4" t="str">
         <f>IF((C302=""),"",VLOOKUP(C302,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20273,7 +20280,7 @@
         <v>11</v>
       </c>
       <c r="D303" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E303" s="4" t="str">
         <f>IF((C303=""),"",VLOOKUP(C303,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20315,7 +20322,7 @@
         <v>11</v>
       </c>
       <c r="D304" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E304" s="4" t="str">
         <f>IF((C304=""),"",VLOOKUP(C304,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20354,7 +20361,7 @@
         <v>11</v>
       </c>
       <c r="D305" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E305" s="4" t="str">
         <f>IF((C305=""),"",VLOOKUP(C305,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20396,7 +20403,7 @@
         <v>11</v>
       </c>
       <c r="D306" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E306" s="4" t="str">
         <f>IF((C306=""),"",VLOOKUP(C306,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20438,7 +20445,7 @@
         <v>11</v>
       </c>
       <c r="D307" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E307" s="4" t="str">
         <f>IF((C307=""),"",VLOOKUP(C307,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20801,7 +20808,7 @@
         <v>11</v>
       </c>
       <c r="D316" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="E316" s="4" t="str">
         <f>IF((C316=""),"",VLOOKUP(C316,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20843,7 +20850,7 @@
         <v>11</v>
       </c>
       <c r="D317" s="14" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E317" s="4" t="str">
         <f>IF((C317=""),"",VLOOKUP(C317,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20882,7 +20889,7 @@
         <v>12</v>
       </c>
       <c r="D318" s="33" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E318" s="4" t="str">
         <f>IF((C318=""),"",VLOOKUP(C318,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -20960,7 +20967,7 @@
         <v>12</v>
       </c>
       <c r="D320" s="1" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E320" s="4" t="str">
         <f>IF((C320=""),"",VLOOKUP(C320,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21122,7 +21129,7 @@
         <v>12</v>
       </c>
       <c r="D324" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E324" s="4" t="str">
         <f>IF((C324=""),"",VLOOKUP(C324,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21164,7 +21171,7 @@
         <v>12</v>
       </c>
       <c r="D325" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E325" s="4" t="str">
         <f>IF((C325=""),"",VLOOKUP(C325,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21206,7 +21213,7 @@
         <v>12</v>
       </c>
       <c r="D326" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E326" s="4" t="str">
         <f>IF((C326=""),"",VLOOKUP(C326,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21245,7 +21252,7 @@
         <v>12</v>
       </c>
       <c r="D327" s="1" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E327" s="4" t="str">
         <f>IF((C327=""),"",VLOOKUP(C327,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21287,7 +21294,7 @@
         <v>12</v>
       </c>
       <c r="D328" s="14" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E328" s="4" t="str">
         <f>IF((C328=""),"",VLOOKUP(C328,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21329,7 +21336,7 @@
         <v>12</v>
       </c>
       <c r="D329" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E329" s="4" t="str">
         <f>IF((C329=""),"",VLOOKUP(C329,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21530,7 +21537,7 @@
         <v>12</v>
       </c>
       <c r="D334" s="16" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="E334" s="4" t="str">
         <f>IF((C334=""),"",VLOOKUP(C334,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -21572,7 +21579,7 @@
         <v>12</v>
       </c>
       <c r="D335" s="14" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E335" s="4" t="str">
         <f>IF((C335=""),"",VLOOKUP(C335,[1]Phases!$A$2:$B$13,2,FALSE))</f>
@@ -22230,7 +22237,7 @@
         <v>Federal Involvement Determination</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="E31" s="2">
         <v>36</v>
@@ -22248,7 +22255,7 @@
         <v>Federal Involvement Determination</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E32" s="2">
         <v>37</v>
@@ -22266,7 +22273,7 @@
         <v>Federal Involvement Determination</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E33" s="2">
         <v>38</v>
@@ -22302,7 +22309,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E35" s="2">
         <v>40</v>
@@ -22320,7 +22327,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D36" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E36" s="2">
         <v>41</v>
@@ -22338,7 +22345,7 @@
         <v>Process Order Issued &amp; Regulatory Coordination Plan Posted</v>
       </c>
       <c r="D37" s="30" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E37" s="2">
         <v>42</v>
@@ -22410,7 +22417,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E41" s="2">
         <v>46</v>
@@ -22428,7 +22435,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D42" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E42" s="2">
         <v>47</v>
@@ -22464,7 +22471,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E44" s="2">
         <v>49</v>
@@ -22482,7 +22489,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D45" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E45" s="2">
         <v>50</v>
@@ -22500,7 +22507,7 @@
         <v>Notice to Proponent to Prepare Revised EAC Application</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="E46" s="2">
         <v>51</v>
@@ -22572,7 +22579,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E50" s="2">
         <v>55</v>
@@ -22590,7 +22597,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D51" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E51" s="2">
         <v>56</v>
@@ -22608,7 +22615,7 @@
         <v>Revised EAC Application Acceptance Decision (Day Zero)</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E52" s="2">
         <v>57</v>
@@ -22626,7 +22633,7 @@
         <v>Revised EAC Application Acceptance Decision (Day Zero)</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E53" s="2">
         <v>58</v>
@@ -22662,7 +22669,7 @@
         <v>EAC Assessment Terminated s.39(d)</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E55" s="2">
         <v>60</v>
@@ -22680,7 +22687,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D56" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E56" s="2">
         <v>61</v>
@@ -22698,7 +22705,7 @@
         <v>EAC Referral Package sent to Ministers</v>
       </c>
       <c r="D57" s="30" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E57" s="2">
         <v>62</v>
@@ -22716,7 +22723,7 @@
         <v>Project Withdrawn</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E58" s="2">
         <v>63</v>
@@ -22734,7 +22741,7 @@
         <v>EAC Ministers Decision</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E59" s="2">
         <v>64</v>
@@ -22752,7 +22759,7 @@
         <v>EAC Ministers Decision</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E60" s="2">
         <v>65</v>
@@ -22780,11 +22787,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C109" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F69" sqref="F69"/>
+      <selection pane="bottomRight" activeCell="F65" sqref="F65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -22840,7 +22847,7 @@
         <v>170</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G2" s="2">
         <v>1</v>
@@ -22864,7 +22871,7 @@
         <v>170</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G3" s="2">
         <v>2</v>
@@ -22888,7 +22895,7 @@
         <v>172</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G4" s="2">
         <v>3</v>
@@ -22912,7 +22919,7 @@
         <v>174</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G5" s="2">
         <v>4</v>
@@ -22936,7 +22943,7 @@
         <v>176</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G6" s="2">
         <v>5</v>
@@ -22960,7 +22967,7 @@
         <v>178</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G7" s="2">
         <v>6</v>
@@ -22984,7 +22991,7 @@
         <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -23008,7 +23015,7 @@
         <v>181</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -23029,10 +23036,10 @@
         <v>182</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
@@ -23053,7 +23060,10 @@
         <v>183</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>362</v>
+        <v>360</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>363</v>
       </c>
       <c r="G11" s="40">
         <v>11</v>
@@ -23077,7 +23087,7 @@
         <v>185</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G12" s="2">
         <v>12</v>
@@ -23101,7 +23111,7 @@
         <v>172</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G13" s="2">
         <v>13</v>
@@ -23125,7 +23135,7 @@
         <v>174</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G14" s="2">
         <v>14</v>
@@ -23149,7 +23159,7 @@
         <v>186</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G15" s="2">
         <v>15</v>
@@ -23173,7 +23183,7 @@
         <v>178</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G16" s="2">
         <v>16</v>
@@ -23197,7 +23207,7 @@
         <v>172</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G17" s="2">
         <v>17</v>
@@ -23221,7 +23231,7 @@
         <v>174</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G18" s="2">
         <v>18</v>
@@ -23245,7 +23255,7 @@
         <v>176</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G19" s="2">
         <v>19</v>
@@ -23269,7 +23279,7 @@
         <v>178</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G20" s="2">
         <v>20</v>
@@ -23293,7 +23303,7 @@
         <v>187</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G21" s="2">
         <v>21</v>
@@ -23317,7 +23327,7 @@
         <v>170</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G22" s="2">
         <v>22</v>
@@ -23341,7 +23351,7 @@
         <v>170</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G23" s="2">
         <v>23</v>
@@ -23365,7 +23375,7 @@
         <v>172</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G24" s="2">
         <v>24</v>
@@ -23389,7 +23399,7 @@
         <v>174</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G25" s="2">
         <v>25</v>
@@ -23413,7 +23423,7 @@
         <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G26" s="2">
         <v>26</v>
@@ -23437,7 +23447,7 @@
         <v>178</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G27" s="2">
         <v>27</v>
@@ -23461,7 +23471,7 @@
         <v>172</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G28" s="2">
         <v>28</v>
@@ -23485,7 +23495,7 @@
         <v>174</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G29" s="2">
         <v>29</v>
@@ -23509,7 +23519,7 @@
         <v>176</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G30" s="2">
         <v>30</v>
@@ -23533,7 +23543,7 @@
         <v>178</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G31" s="2">
         <v>31</v>
@@ -23557,7 +23567,7 @@
         <v>188</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G32" s="2">
         <v>32</v>
@@ -23578,10 +23588,10 @@
         <v>189</v>
       </c>
       <c r="E33" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F33" s="1" t="s">
         <v>351</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>352</v>
       </c>
       <c r="G33" s="2">
         <v>33</v>
@@ -23605,7 +23615,7 @@
         <v>192</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G34" s="2">
         <v>36</v>
@@ -23629,7 +23639,7 @@
         <v>193</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="G35" s="2">
         <v>37</v>
@@ -23653,7 +23663,7 @@
         <v>170</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G36" s="2">
         <v>38</v>
@@ -23677,7 +23687,7 @@
         <v>185</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G37" s="2">
         <v>39</v>
@@ -23701,7 +23711,7 @@
         <v>172</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G38" s="2">
         <v>40</v>
@@ -23725,7 +23735,7 @@
         <v>174</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G39" s="2">
         <v>41</v>
@@ -23749,7 +23759,7 @@
         <v>186</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G40" s="2">
         <v>42</v>
@@ -23773,7 +23783,7 @@
         <v>178</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G41" s="2">
         <v>43</v>
@@ -23797,7 +23807,7 @@
         <v>172</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G42" s="2">
         <v>44</v>
@@ -23821,7 +23831,7 @@
         <v>174</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G43" s="2">
         <v>45</v>
@@ -23845,7 +23855,7 @@
         <v>176</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G44" s="2">
         <v>46</v>
@@ -23869,7 +23879,7 @@
         <v>178</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G45" s="2">
         <v>47</v>
@@ -23893,7 +23903,7 @@
         <v>194</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="G46" s="2">
         <v>48</v>
@@ -23917,7 +23927,7 @@
         <v>172</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G47" s="2">
         <v>49</v>
@@ -23941,7 +23951,7 @@
         <v>174</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G48" s="2">
         <v>50</v>
@@ -23965,7 +23975,7 @@
         <v>176</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G49" s="2">
         <v>51</v>
@@ -23989,7 +23999,7 @@
         <v>178</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G50" s="2">
         <v>52</v>
@@ -24013,7 +24023,7 @@
         <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G51" s="2">
         <v>53</v>
@@ -24037,7 +24047,7 @@
         <v>197</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G52" s="2">
         <v>54</v>
@@ -24061,7 +24071,7 @@
         <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G53" s="2">
         <v>55</v>
@@ -24085,7 +24095,7 @@
         <v>199</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="G54" s="2">
         <v>56</v>
@@ -24109,7 +24119,7 @@
         <v>185</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G55" s="2">
         <v>57</v>
@@ -24133,7 +24143,7 @@
         <v>172</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G56" s="2">
         <v>58</v>
@@ -24157,7 +24167,7 @@
         <v>174</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G57" s="2">
         <v>59</v>
@@ -24181,7 +24191,7 @@
         <v>186</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G58" s="2">
         <v>60</v>
@@ -24205,7 +24215,7 @@
         <v>178</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G59" s="2">
         <v>61</v>
@@ -24229,7 +24239,7 @@
         <v>172</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G60" s="2">
         <v>62</v>
@@ -24253,7 +24263,7 @@
         <v>174</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G61" s="2">
         <v>63</v>
@@ -24277,7 +24287,7 @@
         <v>176</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G62" s="2">
         <v>64</v>
@@ -24301,7 +24311,7 @@
         <v>178</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G63" s="2">
         <v>65</v>
@@ -24322,10 +24332,10 @@
         <v>189</v>
       </c>
       <c r="E64" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="F64" s="30" t="s">
         <v>351</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>352</v>
       </c>
       <c r="G64" s="2">
         <v>66</v>
@@ -24348,8 +24358,8 @@
       <c r="E65" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F65" s="30" t="s">
-        <v>358</v>
+      <c r="F65" s="43" t="s">
+        <v>352</v>
       </c>
       <c r="G65" s="2">
         <v>69</v>
@@ -24370,10 +24380,10 @@
         <v>189</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G66" s="2">
         <v>70</v>
@@ -24397,7 +24407,7 @@
         <v>190</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G67" s="2">
         <v>78</v>
@@ -24421,7 +24431,7 @@
         <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="G68" s="2">
         <v>79</v>
@@ -24445,7 +24455,7 @@
         <v>201</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G69" s="38">
         <v>80</v>
@@ -24469,7 +24479,7 @@
         <v>200</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G70" s="2">
         <v>82</v>
@@ -24493,7 +24503,7 @@
         <v>202</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G71" s="2">
         <v>88</v>
@@ -24514,10 +24524,10 @@
         <v>226</v>
       </c>
       <c r="E72" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="F72" s="1" t="s">
         <v>320</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>321</v>
       </c>
       <c r="G72" s="2">
         <v>96</v>
@@ -24538,10 +24548,10 @@
         <v>226</v>
       </c>
       <c r="E73" s="30" t="s">
+        <v>321</v>
+      </c>
+      <c r="F73" s="1" t="s">
         <v>322</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>323</v>
       </c>
       <c r="G73" s="2">
         <v>97</v>
@@ -24565,7 +24575,7 @@
         <v>202</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G74" s="2">
         <v>98</v>
@@ -24589,7 +24599,7 @@
         <v>185</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G75" s="2">
         <v>99</v>
@@ -24613,7 +24623,7 @@
         <v>172</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G76" s="2">
         <v>100</v>
@@ -24637,7 +24647,7 @@
         <v>174</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G77" s="2">
         <v>101</v>
@@ -24661,7 +24671,7 @@
         <v>186</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G78" s="2">
         <v>102</v>
@@ -24685,7 +24695,7 @@
         <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G79" s="2">
         <v>103</v>
@@ -24709,7 +24719,7 @@
         <v>172</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G80" s="2">
         <v>104</v>
@@ -24733,7 +24743,7 @@
         <v>174</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G81" s="2">
         <v>105</v>
@@ -24757,7 +24767,7 @@
         <v>176</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G82" s="2">
         <v>106</v>
@@ -24781,7 +24791,7 @@
         <v>178</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G83" s="2">
         <v>107</v>
@@ -24802,10 +24812,10 @@
         <v>191</v>
       </c>
       <c r="E84" s="30" t="s">
+        <v>330</v>
+      </c>
+      <c r="F84" s="30" t="s">
         <v>331</v>
-      </c>
-      <c r="F84" s="30" t="s">
-        <v>332</v>
       </c>
       <c r="G84" s="2">
         <v>108</v>
@@ -24829,7 +24839,7 @@
         <v>170</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G85" s="2">
         <v>109</v>
@@ -24853,7 +24863,7 @@
         <v>170</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G86" s="2">
         <v>110</v>
@@ -24877,7 +24887,7 @@
         <v>185</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G87" s="2">
         <v>111</v>
@@ -24901,7 +24911,7 @@
         <v>172</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G88" s="2">
         <v>112</v>
@@ -24925,7 +24935,7 @@
         <v>174</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G89" s="2">
         <v>113</v>
@@ -24949,7 +24959,7 @@
         <v>186</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G90" s="2">
         <v>114</v>
@@ -24973,7 +24983,7 @@
         <v>178</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G91" s="2">
         <v>115</v>
@@ -24997,7 +25007,7 @@
         <v>172</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G92" s="2">
         <v>116</v>
@@ -25021,7 +25031,7 @@
         <v>174</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G93" s="2">
         <v>117</v>
@@ -25045,7 +25055,7 @@
         <v>176</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G94" s="2">
         <v>118</v>
@@ -25069,7 +25079,7 @@
         <v>178</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G95" s="2">
         <v>119</v>
@@ -25093,7 +25103,7 @@
         <v>185</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G96" s="2">
         <v>120</v>
@@ -25117,7 +25127,7 @@
         <v>172</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G97" s="2">
         <v>121</v>
@@ -25141,7 +25151,7 @@
         <v>174</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G98" s="2">
         <v>122</v>
@@ -25165,7 +25175,7 @@
         <v>186</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G99" s="2">
         <v>123</v>
@@ -25189,7 +25199,7 @@
         <v>178</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G100" s="2">
         <v>124</v>
@@ -25213,7 +25223,7 @@
         <v>172</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G101" s="2">
         <v>125</v>
@@ -25237,7 +25247,7 @@
         <v>174</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G102" s="2">
         <v>126</v>
@@ -25261,7 +25271,7 @@
         <v>176</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G103" s="2">
         <v>127</v>
@@ -25285,7 +25295,7 @@
         <v>178</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G104" s="2">
         <v>128</v>
@@ -25306,10 +25316,10 @@
         <v>191</v>
       </c>
       <c r="E105" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="F105" s="30" t="s">
         <v>333</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>334</v>
       </c>
       <c r="G105" s="2">
         <v>129</v>
@@ -25333,7 +25343,7 @@
         <v>170</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G106" s="2">
         <v>130</v>
@@ -25357,7 +25367,7 @@
         <v>170</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G107" s="2">
         <v>131</v>
@@ -25381,7 +25391,7 @@
         <v>185</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G108" s="2">
         <v>132</v>
@@ -25405,7 +25415,7 @@
         <v>172</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G109" s="2">
         <v>133</v>
@@ -25429,7 +25439,7 @@
         <v>174</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G110" s="2">
         <v>134</v>
@@ -25453,7 +25463,7 @@
         <v>186</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G111" s="2">
         <v>135</v>
@@ -25477,7 +25487,7 @@
         <v>178</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G112" s="2">
         <v>136</v>
@@ -25501,7 +25511,7 @@
         <v>172</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G113" s="2">
         <v>137</v>
@@ -25525,7 +25535,7 @@
         <v>174</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G114" s="2">
         <v>138</v>
@@ -25549,7 +25559,7 @@
         <v>176</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G115" s="2">
         <v>139</v>
@@ -25573,7 +25583,7 @@
         <v>178</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G116" s="2">
         <v>140</v>
@@ -25594,10 +25604,10 @@
         <v>191</v>
       </c>
       <c r="E117" s="30" t="s">
+        <v>334</v>
+      </c>
+      <c r="F117" s="30" t="s">
         <v>335</v>
-      </c>
-      <c r="F117" s="30" t="s">
-        <v>336</v>
       </c>
       <c r="G117" s="2">
         <v>141</v>
@@ -25618,10 +25628,10 @@
         <v>182</v>
       </c>
       <c r="E118" s="30" t="s">
+        <v>336</v>
+      </c>
+      <c r="F118" s="1" t="s">
         <v>337</v>
-      </c>
-      <c r="F118" s="1" t="s">
-        <v>338</v>
       </c>
       <c r="G118" s="2">
         <v>142</v>
@@ -25642,10 +25652,10 @@
         <v>183</v>
       </c>
       <c r="E119" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="F119" s="1" t="s">
         <v>339</v>
-      </c>
-      <c r="F119" s="1" t="s">
-        <v>340</v>
       </c>
       <c r="G119" s="2">
         <v>143</v>
@@ -25669,7 +25679,7 @@
         <v>185</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="G120" s="2">
         <v>144</v>
@@ -25693,7 +25703,7 @@
         <v>172</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G121" s="2">
         <v>145</v>
@@ -25717,7 +25727,7 @@
         <v>174</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G122" s="2">
         <v>146</v>
@@ -25741,7 +25751,7 @@
         <v>186</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G123" s="2">
         <v>147</v>
@@ -25765,7 +25775,7 @@
         <v>178</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G124" s="2">
         <v>148</v>
@@ -25789,7 +25799,7 @@
         <v>172</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G125" s="2">
         <v>149</v>
@@ -25813,7 +25823,7 @@
         <v>174</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G126" s="2">
         <v>150</v>
@@ -25837,7 +25847,7 @@
         <v>176</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G127" s="2">
         <v>151</v>
@@ -25861,7 +25871,7 @@
         <v>178</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G128" s="2">
         <v>152</v>
@@ -25882,10 +25892,10 @@
         <v>191</v>
       </c>
       <c r="E129" s="30" t="s">
+        <v>340</v>
+      </c>
+      <c r="F129" s="30" t="s">
         <v>341</v>
-      </c>
-      <c r="F129" s="30" t="s">
-        <v>342</v>
       </c>
       <c r="G129" s="2">
         <v>153</v>
@@ -25909,7 +25919,7 @@
         <v>172</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G130" s="2">
         <v>154</v>
@@ -25933,7 +25943,7 @@
         <v>174</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G131" s="2">
         <v>155</v>
@@ -25957,7 +25967,7 @@
         <v>176</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G132" s="2">
         <v>156</v>
@@ -25981,7 +25991,7 @@
         <v>178</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G133" s="2">
         <v>157</v>
@@ -26005,7 +26015,7 @@
         <v>195</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G134" s="2">
         <v>158</v>
@@ -26029,7 +26039,7 @@
         <v>197</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G135" s="2">
         <v>159</v>
@@ -26053,7 +26063,7 @@
         <v>195</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G136" s="2">
         <v>160</v>
@@ -26077,7 +26087,7 @@
         <v>178</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G137" s="2">
         <v>161</v>
@@ -27780,14 +27790,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28020,21 +28028,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28059,9 +28066,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixes-actions, eventform decision box, exemption template
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BD7687-9093-445A-9DAD-3822919D9609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8EAE0B-7154-4928-B5D9-C38E73187ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="366">
   <si>
     <t>No</t>
   </si>
@@ -1045,39 +1045,21 @@
     <t>Set "EAC Application Development (Proponent Time)| Start of EAC Application Development" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of EAC Application Development", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Set "Revised EAC Application Development (Proponent Time) | Start of Revised EAC Application Development" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of Revised EAC Application Development", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Set "Effects Assessment &amp; Recommendation | Start of Effects Assessment (Day One)" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"Effects Assessment &amp; Recommendation","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of Effects Assessment (Day One)", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Add EVENT "Revised EAC Application Development (Proponent Time) | Submission of Updated Revised EAC Application for Acceptance" at thisEvent ACTUAL +28  (a renamed copy of original EVENT),Add EVENT "Revised EAC Application Development (Proponent Time) | Updated Revised EAC Application Acceptance Decision (Day Zero)" at thisEvent ACTUAL +88  (a renamed copy of original EVENT)</t>
   </si>
   <si>
-    <t>[{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Submission of Revised EAC Application for CEAO Acceptance", "start_at": 28 },{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)", "start_at": 60 }]</t>
-  </si>
-  <si>
     <t>Set "Revised EAC Application Development (Proponent Time) | Updated Revised EAC Application Acceptance Decision (Day Zero)" to PHASE END EVENT</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)"}</t>
-  </si>
-  <si>
     <t>Set "EAC Decision | EAC Referral Package Received by Ministers" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"EAC Decision","work_type_id": 6, "ea_act_id": 3, "event_name": "EAC Referral Package Received by Ministers", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>{"work_state": "COMPLETED"}</t>
   </si>
   <si>
@@ -1102,9 +1084,6 @@
     <t>{"phase_name":"Revised DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of DPD Development", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of DPD Development"}</t>
-  </si>
-  <si>
     <t>{"phase_name":"Exemption Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Package Received by Minister", "start_at": 1 }</t>
   </si>
   <si>
@@ -1141,22 +1120,53 @@
     <t>{"phase_name":"Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 1 }</t>
   </si>
   <si>
-    <t>[{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of IPD/EP for CEAO Approval", "start_at": 28 },{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)", "start_at": 10 }]</t>
-  </si>
-  <si>
     <t>[{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Package Referred to Minister", "is_active": false },{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Last Day of Readiness Decision (Exemption Request)", "is_active": false }]</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of IPD/EP for CEAO Approval", "start_at": 28 },{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)", "start_at": 10 }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of EAC Application Development", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of Revised EAC Application Development", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Effects Assessment &amp; Recommendation","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of Effects Assessment (Day One)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of Revised EAC Application for CEAO Acceptance", "start_at": 28 },{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)", "start_at": 60 }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)"}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"EAC Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Referral Package Received by Ministers", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "CEAO's Readiness Decision (Exemption Request)"}</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Further Readiness Decision", "legislated": false }]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1325,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1342,14 +1352,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1358,7 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1370,13 +1380,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1385,20 +1395,20 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1407,34 +1417,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1444,10 +1451,22 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2944,7 +2963,6 @@
           <cell r="A108">
             <v>106</v>
           </cell>
-          <cell r="B108"/>
           <cell r="C108">
             <v>4</v>
           </cell>
@@ -2956,7 +2974,6 @@
           <cell r="A109">
             <v>107</v>
           </cell>
-          <cell r="B109"/>
           <cell r="C109">
             <v>4</v>
           </cell>
@@ -3242,7 +3259,6 @@
           <cell r="A133">
             <v>131</v>
           </cell>
-          <cell r="B133"/>
           <cell r="C133">
             <v>6</v>
           </cell>
@@ -6729,10 +6745,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7002,7 +7018,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8:C13"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -8001,10 +8017,10 @@
   <dimension ref="A1:M335"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D101" sqref="D101:D118"/>
+      <selection pane="bottomRight" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -13293,7 +13309,7 @@
         <v>6</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E131" s="4" t="str">
         <f>IF((C131=""),"",VLOOKUP(C131,Phases!$A$2:$B$7,2,FALSE))</f>
@@ -21677,10 +21693,10 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -21709,7 +21725,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -21729,7 +21745,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="41"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
@@ -21748,6 +21764,7 @@
       <c r="E3" s="2">
         <v>2</v>
       </c>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
@@ -21784,7 +21801,7 @@
       <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
@@ -21803,6 +21820,7 @@
       <c r="E6" s="2">
         <v>5</v>
       </c>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
@@ -21875,7 +21893,7 @@
       <c r="E10" s="2">
         <v>9</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
@@ -21966,6 +21984,7 @@
       <c r="E15" s="2">
         <v>14</v>
       </c>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
@@ -22056,7 +22075,7 @@
       <c r="E20" s="2">
         <v>19</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
@@ -22093,7 +22112,7 @@
       <c r="E22" s="2">
         <v>21</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
@@ -22112,6 +22131,7 @@
       <c r="E23" s="2">
         <v>22</v>
       </c>
+      <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
@@ -22202,6 +22222,7 @@
       <c r="E28" s="2">
         <v>27</v>
       </c>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
@@ -22802,10 +22823,10 @@
   <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomRight" activeCell="B53" sqref="B53:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -23005,7 +23026,7 @@
         <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -23029,7 +23050,7 @@
         <v>181</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -23050,36 +23071,36 @@
         <v>182</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="41" customFormat="1">
-      <c r="A11" s="40">
+    <row r="11" spans="1:7" s="40" customFormat="1">
+      <c r="A11" s="39">
         <v>11</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="39">
         <v>5</v>
       </c>
-      <c r="C11" s="41" t="str">
+      <c r="C11" s="40" t="str">
         <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised IPD/EP - s.13(3)(b)</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>357</v>
+      <c r="E11" s="41" t="s">
+        <v>350</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="G11" s="40">
+        <v>353</v>
+      </c>
+      <c r="G11" s="39">
         <v>11</v>
       </c>
     </row>
@@ -23317,7 +23338,7 @@
         <v>187</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G21" s="2">
         <v>21</v>
@@ -23565,7 +23586,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3">
         <v>14</v>
@@ -23574,11 +23595,11 @@
         <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
-      <c r="D32" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>188</v>
+      <c r="D32" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>193</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>364</v>
@@ -23587,33 +23608,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="2">
-        <v>33</v>
-      </c>
-      <c r="B33" s="3">
+    <row r="33" spans="1:7" s="44" customFormat="1">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15">
         <v>14</v>
       </c>
-      <c r="C33" s="4" t="str">
+      <c r="C33" s="44" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="G33" s="2">
+      <c r="D33" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="G33" s="15">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>14</v>
@@ -23623,21 +23644,21 @@
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>192</v>
+        <v>341</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="G34" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="3">
         <v>14</v>
@@ -23647,16 +23668,16 @@
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="G35" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -23680,7 +23701,7 @@
         <v>323</v>
       </c>
       <c r="G36" s="2">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -23704,7 +23725,7 @@
         <v>324</v>
       </c>
       <c r="G37" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -23728,7 +23749,7 @@
         <v>325</v>
       </c>
       <c r="G38" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -23752,7 +23773,7 @@
         <v>326</v>
       </c>
       <c r="G39" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -23776,7 +23797,7 @@
         <v>327</v>
       </c>
       <c r="G40" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -23800,7 +23821,7 @@
         <v>328</v>
       </c>
       <c r="G41" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -23824,7 +23845,7 @@
         <v>325</v>
       </c>
       <c r="G42" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -23848,7 +23869,7 @@
         <v>326</v>
       </c>
       <c r="G43" s="2">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -23872,7 +23893,7 @@
         <v>329</v>
       </c>
       <c r="G44" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -23896,7 +23917,7 @@
         <v>328</v>
       </c>
       <c r="G45" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -23917,10 +23938,10 @@
         <v>194</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="G46" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -23944,7 +23965,7 @@
         <v>325</v>
       </c>
       <c r="G47" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -23968,7 +23989,7 @@
         <v>326</v>
       </c>
       <c r="G48" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -23992,7 +24013,7 @@
         <v>329</v>
       </c>
       <c r="G49" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -24016,7 +24037,7 @@
         <v>328</v>
       </c>
       <c r="G50" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -24037,10 +24058,10 @@
         <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G51" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -24061,10 +24082,10 @@
         <v>197</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G52" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -24079,16 +24100,16 @@
         <v>Refer the Project to the CEAO for Further Decision</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E53" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="43" t="s">
         <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="G53" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -24109,10 +24130,10 @@
         <v>199</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="G54" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -24136,7 +24157,7 @@
         <v>324</v>
       </c>
       <c r="G55" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -24160,7 +24181,7 @@
         <v>325</v>
       </c>
       <c r="G56" s="2">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -24184,7 +24205,7 @@
         <v>326</v>
       </c>
       <c r="G57" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -24208,7 +24229,7 @@
         <v>327</v>
       </c>
       <c r="G58" s="2">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -24232,7 +24253,7 @@
         <v>328</v>
       </c>
       <c r="G59" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -24256,7 +24277,7 @@
         <v>325</v>
       </c>
       <c r="G60" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -24280,7 +24301,7 @@
         <v>326</v>
       </c>
       <c r="G61" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -24304,7 +24325,7 @@
         <v>329</v>
       </c>
       <c r="G62" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -24328,7 +24349,7 @@
         <v>328</v>
       </c>
       <c r="G63" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -24346,13 +24367,13 @@
         <v>189</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>348</v>
+        <v>341</v>
+      </c>
+      <c r="F64" s="43" t="s">
+        <v>342</v>
       </c>
       <c r="G64" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -24372,11 +24393,11 @@
       <c r="E65" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F65" s="43" t="s">
-        <v>349</v>
+      <c r="F65" s="42" t="s">
+        <v>343</v>
       </c>
       <c r="G65" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -24394,13 +24415,13 @@
         <v>189</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G66" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -24415,16 +24436,16 @@
         <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E67" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="43" t="s">
         <v>190</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="G67" s="2">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -24445,13 +24466,13 @@
         <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G68" s="2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="39" customFormat="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="38" customFormat="1">
       <c r="A69" s="2">
         <v>80</v>
       </c>
@@ -24469,10 +24490,10 @@
         <v>201</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="G69" s="38">
-        <v>80</v>
+        <v>352</v>
+      </c>
+      <c r="G69" s="2">
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -24493,10 +24514,10 @@
         <v>200</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G70" s="2">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -24520,7 +24541,7 @@
         <v>323</v>
       </c>
       <c r="G71" s="2">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -24544,7 +24565,7 @@
         <v>320</v>
       </c>
       <c r="G72" s="2">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -24568,7 +24589,7 @@
         <v>322</v>
       </c>
       <c r="G73" s="2">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -24592,7 +24613,7 @@
         <v>323</v>
       </c>
       <c r="G74" s="2">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -24616,7 +24637,7 @@
         <v>324</v>
       </c>
       <c r="G75" s="2">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -24640,7 +24661,7 @@
         <v>325</v>
       </c>
       <c r="G76" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -24664,7 +24685,7 @@
         <v>326</v>
       </c>
       <c r="G77" s="2">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -24688,7 +24709,7 @@
         <v>327</v>
       </c>
       <c r="G78" s="2">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -24712,7 +24733,7 @@
         <v>328</v>
       </c>
       <c r="G79" s="2">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -24736,7 +24757,7 @@
         <v>325</v>
       </c>
       <c r="G80" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -24760,7 +24781,7 @@
         <v>326</v>
       </c>
       <c r="G81" s="2">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -24784,7 +24805,7 @@
         <v>329</v>
       </c>
       <c r="G82" s="2">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -24808,7 +24829,7 @@
         <v>328</v>
       </c>
       <c r="G83" s="2">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -24828,11 +24849,11 @@
       <c r="E84" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="F84" s="30" t="s">
-        <v>331</v>
+      <c r="F84" s="43" t="s">
+        <v>358</v>
       </c>
       <c r="G84" s="2">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -24856,7 +24877,7 @@
         <v>323</v>
       </c>
       <c r="G85" s="2">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -24880,7 +24901,7 @@
         <v>323</v>
       </c>
       <c r="G86" s="2">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -24904,7 +24925,7 @@
         <v>324</v>
       </c>
       <c r="G87" s="2">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -24928,7 +24949,7 @@
         <v>325</v>
       </c>
       <c r="G88" s="2">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -24952,7 +24973,7 @@
         <v>326</v>
       </c>
       <c r="G89" s="2">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -24976,7 +24997,7 @@
         <v>327</v>
       </c>
       <c r="G90" s="2">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -25000,7 +25021,7 @@
         <v>328</v>
       </c>
       <c r="G91" s="2">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -25024,7 +25045,7 @@
         <v>325</v>
       </c>
       <c r="G92" s="2">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -25048,7 +25069,7 @@
         <v>326</v>
       </c>
       <c r="G93" s="2">
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -25072,7 +25093,7 @@
         <v>329</v>
       </c>
       <c r="G94" s="2">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -25096,7 +25117,7 @@
         <v>328</v>
       </c>
       <c r="G95" s="2">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -25120,7 +25141,7 @@
         <v>324</v>
       </c>
       <c r="G96" s="2">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -25144,7 +25165,7 @@
         <v>325</v>
       </c>
       <c r="G97" s="2">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -25168,7 +25189,7 @@
         <v>326</v>
       </c>
       <c r="G98" s="2">
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -25192,7 +25213,7 @@
         <v>327</v>
       </c>
       <c r="G99" s="2">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -25216,7 +25237,7 @@
         <v>328</v>
       </c>
       <c r="G100" s="2">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -25240,7 +25261,7 @@
         <v>325</v>
       </c>
       <c r="G101" s="2">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -25264,7 +25285,7 @@
         <v>326</v>
       </c>
       <c r="G102" s="2">
-        <v>126</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -25288,7 +25309,7 @@
         <v>329</v>
       </c>
       <c r="G103" s="2">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -25312,7 +25333,7 @@
         <v>328</v>
       </c>
       <c r="G104" s="2">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -25330,13 +25351,13 @@
         <v>191</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>332</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>333</v>
+        <v>331</v>
+      </c>
+      <c r="F105" s="43" t="s">
+        <v>359</v>
       </c>
       <c r="G105" s="2">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -25360,7 +25381,7 @@
         <v>323</v>
       </c>
       <c r="G106" s="2">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -25384,7 +25405,7 @@
         <v>323</v>
       </c>
       <c r="G107" s="2">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -25408,7 +25429,7 @@
         <v>324</v>
       </c>
       <c r="G108" s="2">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -25432,7 +25453,7 @@
         <v>325</v>
       </c>
       <c r="G109" s="2">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -25456,7 +25477,7 @@
         <v>326</v>
       </c>
       <c r="G110" s="2">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -25480,7 +25501,7 @@
         <v>327</v>
       </c>
       <c r="G111" s="2">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -25504,7 +25525,7 @@
         <v>328</v>
       </c>
       <c r="G112" s="2">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -25528,7 +25549,7 @@
         <v>325</v>
       </c>
       <c r="G113" s="2">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -25552,7 +25573,7 @@
         <v>326</v>
       </c>
       <c r="G114" s="2">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -25576,7 +25597,7 @@
         <v>329</v>
       </c>
       <c r="G115" s="2">
-        <v>139</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -25600,7 +25621,7 @@
         <v>328</v>
       </c>
       <c r="G116" s="2">
-        <v>140</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -25618,13 +25639,13 @@
         <v>191</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>334</v>
-      </c>
-      <c r="F117" s="30" t="s">
-        <v>335</v>
+        <v>332</v>
+      </c>
+      <c r="F117" s="43" t="s">
+        <v>360</v>
       </c>
       <c r="G117" s="2">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -25642,13 +25663,13 @@
         <v>182</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>337</v>
+        <v>361</v>
       </c>
       <c r="G118" s="2">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -25666,13 +25687,13 @@
         <v>183</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>339</v>
+        <v>362</v>
       </c>
       <c r="G119" s="2">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -25696,7 +25717,7 @@
         <v>324</v>
       </c>
       <c r="G120" s="2">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -25720,7 +25741,7 @@
         <v>325</v>
       </c>
       <c r="G121" s="2">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -25744,7 +25765,7 @@
         <v>326</v>
       </c>
       <c r="G122" s="2">
-        <v>146</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -25768,7 +25789,7 @@
         <v>327</v>
       </c>
       <c r="G123" s="2">
-        <v>147</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -25792,7 +25813,7 @@
         <v>328</v>
       </c>
       <c r="G124" s="2">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -25816,7 +25837,7 @@
         <v>325</v>
       </c>
       <c r="G125" s="2">
-        <v>149</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -25840,7 +25861,7 @@
         <v>326</v>
       </c>
       <c r="G126" s="2">
-        <v>150</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -25864,7 +25885,7 @@
         <v>329</v>
       </c>
       <c r="G127" s="2">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -25888,7 +25909,7 @@
         <v>328</v>
       </c>
       <c r="G128" s="2">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -25906,13 +25927,13 @@
         <v>191</v>
       </c>
       <c r="E129" s="30" t="s">
-        <v>340</v>
-      </c>
-      <c r="F129" s="30" t="s">
-        <v>341</v>
+        <v>335</v>
+      </c>
+      <c r="F129" s="43" t="s">
+        <v>363</v>
       </c>
       <c r="G129" s="2">
-        <v>153</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -25936,7 +25957,7 @@
         <v>325</v>
       </c>
       <c r="G130" s="2">
-        <v>154</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -25960,7 +25981,7 @@
         <v>326</v>
       </c>
       <c r="G131" s="2">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -25984,7 +26005,7 @@
         <v>329</v>
       </c>
       <c r="G132" s="2">
-        <v>156</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -26008,7 +26029,7 @@
         <v>328</v>
       </c>
       <c r="G133" s="2">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -26029,10 +26050,10 @@
         <v>195</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G134" s="2">
-        <v>158</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -26053,10 +26074,10 @@
         <v>197</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G135" s="2">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -26077,10 +26098,10 @@
         <v>195</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G136" s="2">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -26104,7 +26125,7 @@
         <v>328</v>
       </c>
       <c r="G137" s="2">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -26118,7 +26139,7 @@
           <x14:formula1>
             <xm:f>Lookups!$U$3:$U$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D50 D55:D71</xm:sqref>
+          <xm:sqref>D55:D71 D2:D50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
@@ -27804,12 +27825,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28042,20 +28065,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28080,12 +28104,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
fixes-actions, eventform decision box, exemption template (#2039)
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61BD7687-9093-445A-9DAD-3822919D9609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F8EAE0B-7154-4928-B5D9-C38E73187ED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="365">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="366">
   <si>
     <t>No</t>
   </si>
@@ -1045,39 +1045,21 @@
     <t>Set "EAC Application Development (Proponent Time)| Start of EAC Application Development" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of EAC Application Development", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Set "Revised EAC Application Development (Proponent Time) | Start of Revised EAC Application Development" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of Revised EAC Application Development", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Set "Effects Assessment &amp; Recommendation | Start of Effects Assessment (Day One)" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"Effects Assessment &amp; Recommendation","work_type_id": 6, "ea_act_id": 3, "event_name": "Start of Effects Assessment (Day One)", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>Add EVENT "Revised EAC Application Development (Proponent Time) | Submission of Updated Revised EAC Application for Acceptance" at thisEvent ACTUAL +28  (a renamed copy of original EVENT),Add EVENT "Revised EAC Application Development (Proponent Time) | Updated Revised EAC Application Acceptance Decision (Day Zero)" at thisEvent ACTUAL +88  (a renamed copy of original EVENT)</t>
   </si>
   <si>
-    <t>[{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Submission of Revised EAC Application for CEAO Acceptance", "start_at": 28 },{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)", "start_at": 60 }]</t>
-  </si>
-  <si>
     <t>Set "Revised EAC Application Development (Proponent Time) | Updated Revised EAC Application Acceptance Decision (Day Zero)" to PHASE END EVENT</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 6, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)"}</t>
-  </si>
-  <si>
     <t>Set "EAC Decision | EAC Referral Package Received by Ministers" ANTICIPATED to thisEvent ACTUAL +1</t>
   </si>
   <si>
-    <t>{"phase_name":"EAC Decision","work_type_id": 6, "ea_act_id": 3, "event_name": "EAC Referral Package Received by Ministers", "start_at": 1 }</t>
-  </si>
-  <si>
     <t>{"work_state": "COMPLETED"}</t>
   </si>
   <si>
@@ -1102,9 +1084,6 @@
     <t>{"phase_name":"Revised DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of DPD Development", "start_at": 1 }</t>
   </si>
   <si>
-    <t>{"phase_name":"Revised DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of DPD Development"}</t>
-  </si>
-  <si>
     <t>{"phase_name":"Exemption Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Package Received by Minister", "start_at": 1 }</t>
   </si>
   <si>
@@ -1141,22 +1120,53 @@
     <t>{"phase_name":"Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "IPD/EP Approved (Day One)", "start_at": 1 }</t>
   </si>
   <si>
-    <t>[{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of IPD/EP for CEAO Approval", "start_at": 28 },{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 6, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)", "start_at": 10 }]</t>
-  </si>
-  <si>
     <t>[{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Package Referred to Minister", "is_active": false },{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Last Day of Readiness Decision (Exemption Request)", "is_active": false }]</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of IPD/EP for CEAO Approval", "start_at": 28 },{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "IPD/EP Approval Decision (Day Zero)", "start_at": 10 }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of EAC Application Development", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of Revised EAC Application Development", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Effects Assessment &amp; Recommendation","work_type_id": 5, "ea_act_id": 3, "event_name": "Start of Effects Assessment (Day One)", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Submission of Revised EAC Application for CEAO Acceptance", "start_at": 28 },{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)", "start_at": 60 }]</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Revised EAC Application Acceptance Decision (Day Zero)"}</t>
+  </si>
+  <si>
+    <t>{"phase_name":"EAC Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Referral Package Received by Ministers", "start_at": 1 }</t>
+  </si>
+  <si>
+    <t>{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "CEAO's Readiness Decision (Exemption Request)"}</t>
+  </si>
+  <si>
+    <t>[{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Further Readiness Decision", "legislated": false }]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1325,7 +1335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1342,14 +1352,14 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1358,7 +1368,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1370,13 +1380,13 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1385,20 +1395,20 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1407,34 +1417,31 @@
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1444,10 +1451,22 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -2944,7 +2963,6 @@
           <cell r="A108">
             <v>106</v>
           </cell>
-          <cell r="B108"/>
           <cell r="C108">
             <v>4</v>
           </cell>
@@ -2956,7 +2974,6 @@
           <cell r="A109">
             <v>107</v>
           </cell>
-          <cell r="B109"/>
           <cell r="C109">
             <v>4</v>
           </cell>
@@ -3242,7 +3259,6 @@
           <cell r="A133">
             <v>131</v>
           </cell>
-          <cell r="B133"/>
           <cell r="C133">
             <v>6</v>
           </cell>
@@ -6729,10 +6745,10 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7002,7 +7018,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8:C13"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -8001,10 +8017,10 @@
   <dimension ref="A1:M335"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C96" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B113" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D101" sqref="D101:D118"/>
+      <selection pane="bottomRight" activeCell="A132" sqref="A132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -13293,7 +13309,7 @@
         <v>6</v>
       </c>
       <c r="D131" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="E131" s="4" t="str">
         <f>IF((C131=""),"",VLOOKUP(C131,Phases!$A$2:$B$7,2,FALSE))</f>
@@ -21677,10 +21693,10 @@
   <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -21709,7 +21725,7 @@
         <v>8</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -21729,7 +21745,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="F2" s="41"/>
+      <c r="F2" s="40"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2">
@@ -21748,6 +21764,7 @@
       <c r="E3" s="2">
         <v>2</v>
       </c>
+      <c r="F3" s="40"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2">
@@ -21784,7 +21801,7 @@
       <c r="E5" s="2">
         <v>4</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="40"/>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2">
@@ -21803,6 +21820,7 @@
       <c r="E6" s="2">
         <v>5</v>
       </c>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="2">
@@ -21875,7 +21893,7 @@
       <c r="E10" s="2">
         <v>9</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" s="2">
@@ -21966,6 +21984,7 @@
       <c r="E15" s="2">
         <v>14</v>
       </c>
+      <c r="F15" s="40"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="2">
@@ -22056,7 +22075,7 @@
       <c r="E20" s="2">
         <v>19</v>
       </c>
-      <c r="F20" s="41"/>
+      <c r="F20" s="40"/>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="2">
@@ -22093,7 +22112,7 @@
       <c r="E22" s="2">
         <v>21</v>
       </c>
-      <c r="F22" s="41"/>
+      <c r="F22" s="40"/>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="2">
@@ -22112,6 +22131,7 @@
       <c r="E23" s="2">
         <v>22</v>
       </c>
+      <c r="F23" s="40"/>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="2">
@@ -22202,6 +22222,7 @@
       <c r="E28" s="2">
         <v>27</v>
       </c>
+      <c r="F28" s="40"/>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="2">
@@ -22802,10 +22823,10 @@
   <dimension ref="A1:G137"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B33" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F52" sqref="F52"/>
+      <selection pane="bottomRight" activeCell="B53" sqref="B53:E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -23005,7 +23026,7 @@
         <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -23029,7 +23050,7 @@
         <v>181</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -23050,36 +23071,36 @@
         <v>182</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="41" customFormat="1">
-      <c r="A11" s="40">
+    <row r="11" spans="1:7" s="40" customFormat="1">
+      <c r="A11" s="39">
         <v>11</v>
       </c>
-      <c r="B11" s="40">
+      <c r="B11" s="39">
         <v>5</v>
       </c>
-      <c r="C11" s="41" t="str">
+      <c r="C11" s="40" t="str">
         <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised IPD/EP - s.13(3)(b)</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="40" t="s">
         <v>183</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>357</v>
+      <c r="E11" s="41" t="s">
+        <v>350</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="G11" s="40">
+        <v>353</v>
+      </c>
+      <c r="G11" s="39">
         <v>11</v>
       </c>
     </row>
@@ -23317,7 +23338,7 @@
         <v>187</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>346</v>
+        <v>340</v>
       </c>
       <c r="G21" s="2">
         <v>21</v>
@@ -23565,7 +23586,7 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" s="2">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B32" s="3">
         <v>14</v>
@@ -23574,11 +23595,11 @@
         <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
-      <c r="D32" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>188</v>
+      <c r="D32" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>193</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>364</v>
@@ -23587,33 +23608,33 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
-      <c r="A33" s="2">
-        <v>33</v>
-      </c>
-      <c r="B33" s="3">
+    <row r="33" spans="1:7" s="44" customFormat="1">
+      <c r="A33" s="15">
+        <v>32</v>
+      </c>
+      <c r="B33" s="15">
         <v>14</v>
       </c>
-      <c r="C33" s="4" t="str">
+      <c r="C33" s="44" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>348</v>
-      </c>
-      <c r="G33" s="2">
+      <c r="D33" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="46" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>356</v>
+      </c>
+      <c r="G33" s="15">
         <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" s="2">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>14</v>
@@ -23623,21 +23644,21 @@
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>192</v>
+        <v>341</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="G34" s="2">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" s="2">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B35" s="3">
         <v>14</v>
@@ -23647,16 +23668,16 @@
         <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E35" s="26" t="s">
-        <v>193</v>
+        <v>191</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="G35" s="2">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:7">
@@ -23680,7 +23701,7 @@
         <v>323</v>
       </c>
       <c r="G36" s="2">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:7">
@@ -23704,7 +23725,7 @@
         <v>324</v>
       </c>
       <c r="G37" s="2">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="38" spans="1:7">
@@ -23728,7 +23749,7 @@
         <v>325</v>
       </c>
       <c r="G38" s="2">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="1:7">
@@ -23752,7 +23773,7 @@
         <v>326</v>
       </c>
       <c r="G39" s="2">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:7">
@@ -23776,7 +23797,7 @@
         <v>327</v>
       </c>
       <c r="G40" s="2">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:7">
@@ -23800,7 +23821,7 @@
         <v>328</v>
       </c>
       <c r="G41" s="2">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:7">
@@ -23824,7 +23845,7 @@
         <v>325</v>
       </c>
       <c r="G42" s="2">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="43" spans="1:7">
@@ -23848,7 +23869,7 @@
         <v>326</v>
       </c>
       <c r="G43" s="2">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="44" spans="1:7">
@@ -23872,7 +23893,7 @@
         <v>329</v>
       </c>
       <c r="G44" s="2">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:7">
@@ -23896,7 +23917,7 @@
         <v>328</v>
       </c>
       <c r="G45" s="2">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="46" spans="1:7">
@@ -23917,10 +23938,10 @@
         <v>194</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="G46" s="2">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="47" spans="1:7">
@@ -23944,7 +23965,7 @@
         <v>325</v>
       </c>
       <c r="G47" s="2">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:7">
@@ -23968,7 +23989,7 @@
         <v>326</v>
       </c>
       <c r="G48" s="2">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="49" spans="1:7">
@@ -23992,7 +24013,7 @@
         <v>329</v>
       </c>
       <c r="G49" s="2">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="50" spans="1:7">
@@ -24016,7 +24037,7 @@
         <v>328</v>
       </c>
       <c r="G50" s="2">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="51" spans="1:7">
@@ -24037,10 +24058,10 @@
         <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G51" s="2">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -24061,10 +24082,10 @@
         <v>197</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G52" s="2">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="53" spans="1:7">
@@ -24079,16 +24100,16 @@
         <v>Refer the Project to the CEAO for Further Decision</v>
       </c>
       <c r="D53" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E53" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="43" t="s">
         <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>326</v>
+        <v>365</v>
       </c>
       <c r="G53" s="2">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="54" spans="1:7">
@@ -24109,10 +24130,10 @@
         <v>199</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="G54" s="2">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="55" spans="1:7">
@@ -24136,7 +24157,7 @@
         <v>324</v>
       </c>
       <c r="G55" s="2">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="56" spans="1:7">
@@ -24160,7 +24181,7 @@
         <v>325</v>
       </c>
       <c r="G56" s="2">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:7">
@@ -24184,7 +24205,7 @@
         <v>326</v>
       </c>
       <c r="G57" s="2">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="58" spans="1:7">
@@ -24208,7 +24229,7 @@
         <v>327</v>
       </c>
       <c r="G58" s="2">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="59" spans="1:7">
@@ -24232,7 +24253,7 @@
         <v>328</v>
       </c>
       <c r="G59" s="2">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="60" spans="1:7">
@@ -24256,7 +24277,7 @@
         <v>325</v>
       </c>
       <c r="G60" s="2">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="61" spans="1:7">
@@ -24280,7 +24301,7 @@
         <v>326</v>
       </c>
       <c r="G61" s="2">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="62" spans="1:7">
@@ -24304,7 +24325,7 @@
         <v>329</v>
       </c>
       <c r="G62" s="2">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="63" spans="1:7">
@@ -24328,7 +24349,7 @@
         <v>328</v>
       </c>
       <c r="G63" s="2">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="64" spans="1:7">
@@ -24346,13 +24367,13 @@
         <v>189</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F64" s="30" t="s">
-        <v>348</v>
+        <v>341</v>
+      </c>
+      <c r="F64" s="43" t="s">
+        <v>342</v>
       </c>
       <c r="G64" s="2">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="65" spans="1:7">
@@ -24372,11 +24393,11 @@
       <c r="E65" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="F65" s="43" t="s">
-        <v>349</v>
+      <c r="F65" s="42" t="s">
+        <v>343</v>
       </c>
       <c r="G65" s="2">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="66" spans="1:7">
@@ -24394,13 +24415,13 @@
         <v>189</v>
       </c>
       <c r="E66" s="30" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="F66" s="30" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="G66" s="2">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="67" spans="1:7">
@@ -24415,16 +24436,16 @@
         <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="E67" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="43" t="s">
         <v>190</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="G67" s="2">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="68" spans="1:7">
@@ -24445,13 +24466,13 @@
         <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>349</v>
+        <v>343</v>
       </c>
       <c r="G68" s="2">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" s="39" customFormat="1">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" s="38" customFormat="1">
       <c r="A69" s="2">
         <v>80</v>
       </c>
@@ -24469,10 +24490,10 @@
         <v>201</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="G69" s="38">
-        <v>80</v>
+        <v>352</v>
+      </c>
+      <c r="G69" s="2">
+        <v>69</v>
       </c>
     </row>
     <row r="70" spans="1:7">
@@ -24493,10 +24514,10 @@
         <v>200</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="G70" s="2">
-        <v>82</v>
+        <v>70</v>
       </c>
     </row>
     <row r="71" spans="1:7">
@@ -24520,7 +24541,7 @@
         <v>323</v>
       </c>
       <c r="G71" s="2">
-        <v>88</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:7">
@@ -24544,7 +24565,7 @@
         <v>320</v>
       </c>
       <c r="G72" s="2">
-        <v>96</v>
+        <v>72</v>
       </c>
     </row>
     <row r="73" spans="1:7">
@@ -24568,7 +24589,7 @@
         <v>322</v>
       </c>
       <c r="G73" s="2">
-        <v>97</v>
+        <v>73</v>
       </c>
     </row>
     <row r="74" spans="1:7">
@@ -24592,7 +24613,7 @@
         <v>323</v>
       </c>
       <c r="G74" s="2">
-        <v>98</v>
+        <v>74</v>
       </c>
     </row>
     <row r="75" spans="1:7">
@@ -24616,7 +24637,7 @@
         <v>324</v>
       </c>
       <c r="G75" s="2">
-        <v>99</v>
+        <v>75</v>
       </c>
     </row>
     <row r="76" spans="1:7">
@@ -24640,7 +24661,7 @@
         <v>325</v>
       </c>
       <c r="G76" s="2">
-        <v>100</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:7">
@@ -24664,7 +24685,7 @@
         <v>326</v>
       </c>
       <c r="G77" s="2">
-        <v>101</v>
+        <v>77</v>
       </c>
     </row>
     <row r="78" spans="1:7">
@@ -24688,7 +24709,7 @@
         <v>327</v>
       </c>
       <c r="G78" s="2">
-        <v>102</v>
+        <v>78</v>
       </c>
     </row>
     <row r="79" spans="1:7">
@@ -24712,7 +24733,7 @@
         <v>328</v>
       </c>
       <c r="G79" s="2">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="80" spans="1:7">
@@ -24736,7 +24757,7 @@
         <v>325</v>
       </c>
       <c r="G80" s="2">
-        <v>104</v>
+        <v>80</v>
       </c>
     </row>
     <row r="81" spans="1:7">
@@ -24760,7 +24781,7 @@
         <v>326</v>
       </c>
       <c r="G81" s="2">
-        <v>105</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:7">
@@ -24784,7 +24805,7 @@
         <v>329</v>
       </c>
       <c r="G82" s="2">
-        <v>106</v>
+        <v>82</v>
       </c>
     </row>
     <row r="83" spans="1:7">
@@ -24808,7 +24829,7 @@
         <v>328</v>
       </c>
       <c r="G83" s="2">
-        <v>107</v>
+        <v>83</v>
       </c>
     </row>
     <row r="84" spans="1:7">
@@ -24828,11 +24849,11 @@
       <c r="E84" s="30" t="s">
         <v>330</v>
       </c>
-      <c r="F84" s="30" t="s">
-        <v>331</v>
+      <c r="F84" s="43" t="s">
+        <v>358</v>
       </c>
       <c r="G84" s="2">
-        <v>108</v>
+        <v>84</v>
       </c>
     </row>
     <row r="85" spans="1:7">
@@ -24856,7 +24877,7 @@
         <v>323</v>
       </c>
       <c r="G85" s="2">
-        <v>109</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" spans="1:7">
@@ -24880,7 +24901,7 @@
         <v>323</v>
       </c>
       <c r="G86" s="2">
-        <v>110</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:7">
@@ -24904,7 +24925,7 @@
         <v>324</v>
       </c>
       <c r="G87" s="2">
-        <v>111</v>
+        <v>87</v>
       </c>
     </row>
     <row r="88" spans="1:7">
@@ -24928,7 +24949,7 @@
         <v>325</v>
       </c>
       <c r="G88" s="2">
-        <v>112</v>
+        <v>88</v>
       </c>
     </row>
     <row r="89" spans="1:7">
@@ -24952,7 +24973,7 @@
         <v>326</v>
       </c>
       <c r="G89" s="2">
-        <v>113</v>
+        <v>89</v>
       </c>
     </row>
     <row r="90" spans="1:7">
@@ -24976,7 +24997,7 @@
         <v>327</v>
       </c>
       <c r="G90" s="2">
-        <v>114</v>
+        <v>90</v>
       </c>
     </row>
     <row r="91" spans="1:7">
@@ -25000,7 +25021,7 @@
         <v>328</v>
       </c>
       <c r="G91" s="2">
-        <v>115</v>
+        <v>91</v>
       </c>
     </row>
     <row r="92" spans="1:7">
@@ -25024,7 +25045,7 @@
         <v>325</v>
       </c>
       <c r="G92" s="2">
-        <v>116</v>
+        <v>92</v>
       </c>
     </row>
     <row r="93" spans="1:7">
@@ -25048,7 +25069,7 @@
         <v>326</v>
       </c>
       <c r="G93" s="2">
-        <v>117</v>
+        <v>93</v>
       </c>
     </row>
     <row r="94" spans="1:7">
@@ -25072,7 +25093,7 @@
         <v>329</v>
       </c>
       <c r="G94" s="2">
-        <v>118</v>
+        <v>94</v>
       </c>
     </row>
     <row r="95" spans="1:7">
@@ -25096,7 +25117,7 @@
         <v>328</v>
       </c>
       <c r="G95" s="2">
-        <v>119</v>
+        <v>95</v>
       </c>
     </row>
     <row r="96" spans="1:7">
@@ -25120,7 +25141,7 @@
         <v>324</v>
       </c>
       <c r="G96" s="2">
-        <v>120</v>
+        <v>96</v>
       </c>
     </row>
     <row r="97" spans="1:7">
@@ -25144,7 +25165,7 @@
         <v>325</v>
       </c>
       <c r="G97" s="2">
-        <v>121</v>
+        <v>97</v>
       </c>
     </row>
     <row r="98" spans="1:7">
@@ -25168,7 +25189,7 @@
         <v>326</v>
       </c>
       <c r="G98" s="2">
-        <v>122</v>
+        <v>98</v>
       </c>
     </row>
     <row r="99" spans="1:7">
@@ -25192,7 +25213,7 @@
         <v>327</v>
       </c>
       <c r="G99" s="2">
-        <v>123</v>
+        <v>99</v>
       </c>
     </row>
     <row r="100" spans="1:7">
@@ -25216,7 +25237,7 @@
         <v>328</v>
       </c>
       <c r="G100" s="2">
-        <v>124</v>
+        <v>100</v>
       </c>
     </row>
     <row r="101" spans="1:7">
@@ -25240,7 +25261,7 @@
         <v>325</v>
       </c>
       <c r="G101" s="2">
-        <v>125</v>
+        <v>101</v>
       </c>
     </row>
     <row r="102" spans="1:7">
@@ -25264,7 +25285,7 @@
         <v>326</v>
       </c>
       <c r="G102" s="2">
-        <v>126</v>
+        <v>102</v>
       </c>
     </row>
     <row r="103" spans="1:7">
@@ -25288,7 +25309,7 @@
         <v>329</v>
       </c>
       <c r="G103" s="2">
-        <v>127</v>
+        <v>103</v>
       </c>
     </row>
     <row r="104" spans="1:7">
@@ -25312,7 +25333,7 @@
         <v>328</v>
       </c>
       <c r="G104" s="2">
-        <v>128</v>
+        <v>104</v>
       </c>
     </row>
     <row r="105" spans="1:7">
@@ -25330,13 +25351,13 @@
         <v>191</v>
       </c>
       <c r="E105" s="30" t="s">
-        <v>332</v>
-      </c>
-      <c r="F105" s="30" t="s">
-        <v>333</v>
+        <v>331</v>
+      </c>
+      <c r="F105" s="43" t="s">
+        <v>359</v>
       </c>
       <c r="G105" s="2">
-        <v>129</v>
+        <v>105</v>
       </c>
     </row>
     <row r="106" spans="1:7">
@@ -25360,7 +25381,7 @@
         <v>323</v>
       </c>
       <c r="G106" s="2">
-        <v>130</v>
+        <v>106</v>
       </c>
     </row>
     <row r="107" spans="1:7">
@@ -25384,7 +25405,7 @@
         <v>323</v>
       </c>
       <c r="G107" s="2">
-        <v>131</v>
+        <v>107</v>
       </c>
     </row>
     <row r="108" spans="1:7">
@@ -25408,7 +25429,7 @@
         <v>324</v>
       </c>
       <c r="G108" s="2">
-        <v>132</v>
+        <v>108</v>
       </c>
     </row>
     <row r="109" spans="1:7">
@@ -25432,7 +25453,7 @@
         <v>325</v>
       </c>
       <c r="G109" s="2">
-        <v>133</v>
+        <v>109</v>
       </c>
     </row>
     <row r="110" spans="1:7">
@@ -25456,7 +25477,7 @@
         <v>326</v>
       </c>
       <c r="G110" s="2">
-        <v>134</v>
+        <v>110</v>
       </c>
     </row>
     <row r="111" spans="1:7">
@@ -25480,7 +25501,7 @@
         <v>327</v>
       </c>
       <c r="G111" s="2">
-        <v>135</v>
+        <v>111</v>
       </c>
     </row>
     <row r="112" spans="1:7">
@@ -25504,7 +25525,7 @@
         <v>328</v>
       </c>
       <c r="G112" s="2">
-        <v>136</v>
+        <v>112</v>
       </c>
     </row>
     <row r="113" spans="1:7">
@@ -25528,7 +25549,7 @@
         <v>325</v>
       </c>
       <c r="G113" s="2">
-        <v>137</v>
+        <v>113</v>
       </c>
     </row>
     <row r="114" spans="1:7">
@@ -25552,7 +25573,7 @@
         <v>326</v>
       </c>
       <c r="G114" s="2">
-        <v>138</v>
+        <v>114</v>
       </c>
     </row>
     <row r="115" spans="1:7">
@@ -25576,7 +25597,7 @@
         <v>329</v>
       </c>
       <c r="G115" s="2">
-        <v>139</v>
+        <v>115</v>
       </c>
     </row>
     <row r="116" spans="1:7">
@@ -25600,7 +25621,7 @@
         <v>328</v>
       </c>
       <c r="G116" s="2">
-        <v>140</v>
+        <v>116</v>
       </c>
     </row>
     <row r="117" spans="1:7">
@@ -25618,13 +25639,13 @@
         <v>191</v>
       </c>
       <c r="E117" s="30" t="s">
-        <v>334</v>
-      </c>
-      <c r="F117" s="30" t="s">
-        <v>335</v>
+        <v>332</v>
+      </c>
+      <c r="F117" s="43" t="s">
+        <v>360</v>
       </c>
       <c r="G117" s="2">
-        <v>141</v>
+        <v>117</v>
       </c>
     </row>
     <row r="118" spans="1:7">
@@ -25642,13 +25663,13 @@
         <v>182</v>
       </c>
       <c r="E118" s="30" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>337</v>
+        <v>361</v>
       </c>
       <c r="G118" s="2">
-        <v>142</v>
+        <v>118</v>
       </c>
     </row>
     <row r="119" spans="1:7">
@@ -25666,13 +25687,13 @@
         <v>183</v>
       </c>
       <c r="E119" s="30" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>339</v>
+        <v>362</v>
       </c>
       <c r="G119" s="2">
-        <v>143</v>
+        <v>119</v>
       </c>
     </row>
     <row r="120" spans="1:7">
@@ -25696,7 +25717,7 @@
         <v>324</v>
       </c>
       <c r="G120" s="2">
-        <v>144</v>
+        <v>120</v>
       </c>
     </row>
     <row r="121" spans="1:7">
@@ -25720,7 +25741,7 @@
         <v>325</v>
       </c>
       <c r="G121" s="2">
-        <v>145</v>
+        <v>121</v>
       </c>
     </row>
     <row r="122" spans="1:7">
@@ -25744,7 +25765,7 @@
         <v>326</v>
       </c>
       <c r="G122" s="2">
-        <v>146</v>
+        <v>122</v>
       </c>
     </row>
     <row r="123" spans="1:7">
@@ -25768,7 +25789,7 @@
         <v>327</v>
       </c>
       <c r="G123" s="2">
-        <v>147</v>
+        <v>123</v>
       </c>
     </row>
     <row r="124" spans="1:7">
@@ -25792,7 +25813,7 @@
         <v>328</v>
       </c>
       <c r="G124" s="2">
-        <v>148</v>
+        <v>124</v>
       </c>
     </row>
     <row r="125" spans="1:7">
@@ -25816,7 +25837,7 @@
         <v>325</v>
       </c>
       <c r="G125" s="2">
-        <v>149</v>
+        <v>125</v>
       </c>
     </row>
     <row r="126" spans="1:7">
@@ -25840,7 +25861,7 @@
         <v>326</v>
       </c>
       <c r="G126" s="2">
-        <v>150</v>
+        <v>126</v>
       </c>
     </row>
     <row r="127" spans="1:7">
@@ -25864,7 +25885,7 @@
         <v>329</v>
       </c>
       <c r="G127" s="2">
-        <v>151</v>
+        <v>127</v>
       </c>
     </row>
     <row r="128" spans="1:7">
@@ -25888,7 +25909,7 @@
         <v>328</v>
       </c>
       <c r="G128" s="2">
-        <v>152</v>
+        <v>128</v>
       </c>
     </row>
     <row r="129" spans="1:7">
@@ -25906,13 +25927,13 @@
         <v>191</v>
       </c>
       <c r="E129" s="30" t="s">
-        <v>340</v>
-      </c>
-      <c r="F129" s="30" t="s">
-        <v>341</v>
+        <v>335</v>
+      </c>
+      <c r="F129" s="43" t="s">
+        <v>363</v>
       </c>
       <c r="G129" s="2">
-        <v>153</v>
+        <v>129</v>
       </c>
     </row>
     <row r="130" spans="1:7">
@@ -25936,7 +25957,7 @@
         <v>325</v>
       </c>
       <c r="G130" s="2">
-        <v>154</v>
+        <v>130</v>
       </c>
     </row>
     <row r="131" spans="1:7">
@@ -25960,7 +25981,7 @@
         <v>326</v>
       </c>
       <c r="G131" s="2">
-        <v>155</v>
+        <v>131</v>
       </c>
     </row>
     <row r="132" spans="1:7">
@@ -25984,7 +26005,7 @@
         <v>329</v>
       </c>
       <c r="G132" s="2">
-        <v>156</v>
+        <v>132</v>
       </c>
     </row>
     <row r="133" spans="1:7">
@@ -26008,7 +26029,7 @@
         <v>328</v>
       </c>
       <c r="G133" s="2">
-        <v>157</v>
+        <v>133</v>
       </c>
     </row>
     <row r="134" spans="1:7">
@@ -26029,10 +26050,10 @@
         <v>195</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G134" s="2">
-        <v>158</v>
+        <v>134</v>
       </c>
     </row>
     <row r="135" spans="1:7">
@@ -26053,10 +26074,10 @@
         <v>197</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="G135" s="2">
-        <v>159</v>
+        <v>135</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -26077,10 +26098,10 @@
         <v>195</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="G136" s="2">
-        <v>160</v>
+        <v>136</v>
       </c>
     </row>
     <row r="137" spans="1:7">
@@ -26104,7 +26125,7 @@
         <v>328</v>
       </c>
       <c r="G137" s="2">
-        <v>161</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -26118,7 +26139,7 @@
           <x14:formula1>
             <xm:f>Lookups!$U$3:$U$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D50 D55:D71</xm:sqref>
+          <xm:sqref>D55:D71 D2:D50</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
@@ -27804,12 +27825,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -28042,20 +28065,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -28080,12 +28104,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
work start date per start event and phaes change
</commit_message>
<xml_diff>
--- a/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
+++ b/epictrack-api/src/api/templates/event_templates/exemption_request/002_Exemption_Request.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\epic\track\code\epictrack-api\src\api\templates\event_templates\exemption_request\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90FA236-4C7A-417D-9814-D7DCC88FA611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FC8B2E-BF2E-4591-98DA-C883287F2245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Phases" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$A$1:$G$158</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Actions!$A$1:$G$137</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Events!$A$1:$M$335</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Outcomes!$A$1:$E$15</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2441" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2378" uniqueCount="366">
   <si>
     <t>No</t>
   </si>
@@ -1148,69 +1148,6 @@
   </si>
   <si>
     <t>[{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "new_name": "Further Readiness Decision", "legislated": false }]</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Pre-EA (Exemption Request)","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Early Engagement","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"DPD Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Exemption Request Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Exemption Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Further Readiness Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Assessment Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Process Planning","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Assessment Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Process Planning","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Assessment Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"EAC Application Review","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Assessment Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"EAC Application Review","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Assessment Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Revised EAC Application Development (Proponent Time)","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Effects Assessment &amp; Recommendation","work_type_id": 5, "ea_act_id": 3, "event_name": "EAC Assessment Terminated s.39(d)"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"Effects Assessment &amp; Recommendation","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
-  </si>
-  <si>
-    <t>{"phase_name":"EAC Decision","work_type_id": 5, "ea_act_id": 3, "event_name": "Project Withdrawn"}</t>
   </si>
 </sst>
 </file>
@@ -21765,7 +21702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
@@ -22897,13 +22834,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:G158"/>
+  <dimension ref="A1:G137"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2:G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5"/>
@@ -23090,20 +23027,20 @@
         <v>7</v>
       </c>
       <c r="B8" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C8" s="4" t="str">
         <f>IF((B8=""),"",VLOOKUP(B8,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="26" t="s">
-        <v>193</v>
+        <v>CEAO Approves Submitted IPD/EP - s.13(3)(a)</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>366</v>
+        <v>338</v>
       </c>
       <c r="G8" s="2">
         <v>7</v>
@@ -23121,13 +23058,13 @@
         <v>CEAO Approves Submitted IPD/EP - s.13(3)(a)</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>338</v>
+        <v>355</v>
       </c>
       <c r="G9" s="2">
         <v>8</v>
@@ -23138,68 +23075,68 @@
         <v>9</v>
       </c>
       <c r="B10" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C10" s="4" t="str">
         <f>IF((B10=""),"",VLOOKUP(B10,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Approves Submitted IPD/EP - s.13(3)(a)</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>191</v>
+        <v>CEAO Requires the Proponent to Submit a Revised IPD/EP - s.13(3)(b)</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>182</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>181</v>
+        <v>339</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="G10" s="2">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" s="39" customFormat="1">
       <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="38">
         <v>5</v>
       </c>
-      <c r="C11" s="4" t="str">
+      <c r="C11" s="39" t="str">
         <f>IF((B11=""),"",VLOOKUP(B11,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>CEAO Requires the Proponent to Submit a Revised IPD/EP - s.13(3)(b)</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>339</v>
+      <c r="D11" s="39" t="s">
+        <v>183</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>350</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="G11" s="2">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="39" customFormat="1">
+    <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="38">
-        <v>5</v>
-      </c>
-      <c r="C12" s="39" t="str">
+      <c r="B12" s="3">
+        <v>6</v>
+      </c>
+      <c r="C12" s="4" t="str">
         <f>IF((B12=""),"",VLOOKUP(B12,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised IPD/EP - s.13(3)(b)</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>183</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>350</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>353</v>
+        <v>324</v>
       </c>
       <c r="G12" s="2">
         <v>11</v>
@@ -23210,20 +23147,20 @@
         <v>12</v>
       </c>
       <c r="B13" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C13" s="4" t="str">
         <f>IF((B13=""),"",VLOOKUP(B13,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>184</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D13" t="s">
+        <v>171</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G13" s="2">
         <v>12</v>
@@ -23240,14 +23177,14 @@
         <f>IF((B14=""),"",VLOOKUP(B14,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
-      <c r="D14" t="s">
-        <v>171</v>
+      <c r="D14" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G14" s="2">
         <v>13</v>
@@ -23265,13 +23202,13 @@
         <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G15" s="2">
         <v>14</v>
@@ -23289,13 +23226,13 @@
         <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G16" s="2">
         <v>15</v>
@@ -23306,20 +23243,20 @@
         <v>16</v>
       </c>
       <c r="B17" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="4" t="str">
         <f>IF((B17=""),"",VLOOKUP(B17,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>177</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D17" t="s">
+        <v>171</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="G17" s="2">
         <v>16</v>
@@ -23330,20 +23267,20 @@
         <v>17</v>
       </c>
       <c r="B18" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C18" s="4" t="str">
         <f>IF((B18=""),"",VLOOKUP(B18,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>193</v>
+        <v>173</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>368</v>
+        <v>326</v>
       </c>
       <c r="G18" s="2">
         <v>17</v>
@@ -23360,14 +23297,14 @@
         <f>IF((B19=""),"",VLOOKUP(B19,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
-      <c r="D19" t="s">
-        <v>171</v>
+      <c r="D19" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="G19" s="2">
         <v>18</v>
@@ -23385,13 +23322,13 @@
         <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G20" s="2">
         <v>19</v>
@@ -23402,20 +23339,20 @@
         <v>20</v>
       </c>
       <c r="B21" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C21" s="4" t="str">
         <f>IF((B21=""),"",VLOOKUP(B21,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D21" s="9" t="s">
-        <v>175</v>
+        <v>Last Day of Exemption Request: Early Engagement PHASE</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>176</v>
+        <v>187</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>329</v>
+        <v>340</v>
       </c>
       <c r="G21" s="2">
         <v>20</v>
@@ -23426,20 +23363,20 @@
         <v>21</v>
       </c>
       <c r="B22" s="3">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C22" s="4" t="str">
         <f>IF((B22=""),"",VLOOKUP(B22,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>177</v>
+        <v>EAO's Viewpoint is POSITIVE</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G22" s="2">
         <v>21</v>
@@ -23450,20 +23387,20 @@
         <v>22</v>
       </c>
       <c r="B23" s="3">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="C23" s="4" t="str">
         <f>IF((B23=""),"",VLOOKUP(B23,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E23" s="26" t="s">
-        <v>193</v>
+        <v>EAO's Viewpoint is NEGATIVE</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>367</v>
+        <v>323</v>
       </c>
       <c r="G23" s="2">
         <v>22</v>
@@ -23474,20 +23411,20 @@
         <v>23</v>
       </c>
       <c r="B24" s="3">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C24" s="4" t="str">
         <f>IF((B24=""),"",VLOOKUP(B24,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Last Day of Exemption Request: Early Engagement PHASE</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>191</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D24" t="s">
+        <v>171</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>187</v>
+        <v>172</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="G24" s="2">
         <v>23</v>
@@ -23498,20 +23435,20 @@
         <v>24</v>
       </c>
       <c r="B25" s="3">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C25" s="4" t="str">
         <f>IF((B25=""),"",VLOOKUP(B25,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>EAO's Viewpoint is POSITIVE</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>169</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G25" s="2">
         <v>24</v>
@@ -23522,20 +23459,20 @@
         <v>25</v>
       </c>
       <c r="B26" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C26" s="4" t="str">
         <f>IF((B26=""),"",VLOOKUP(B26,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>EAO's Viewpoint is NEGATIVE</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>169</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="G26" s="2">
         <v>25</v>
@@ -23552,14 +23489,14 @@
         <f>IF((B27=""),"",VLOOKUP(B27,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
-      <c r="D27" t="s">
-        <v>171</v>
+      <c r="D27" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G27" s="2">
         <v>26</v>
@@ -23570,20 +23507,20 @@
         <v>27</v>
       </c>
       <c r="B28" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C28" s="4" t="str">
         <f>IF((B28=""),"",VLOOKUP(B28,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D28" s="9" t="s">
-        <v>173</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D28" t="s">
+        <v>171</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G28" s="2">
         <v>27</v>
@@ -23594,20 +23531,20 @@
         <v>28</v>
       </c>
       <c r="B29" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C29" s="4" t="str">
         <f>IF((B29=""),"",VLOOKUP(B29,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G29" s="2">
         <v>28</v>
@@ -23618,20 +23555,20 @@
         <v>29</v>
       </c>
       <c r="B30" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C30" s="4" t="str">
         <f>IF((B30=""),"",VLOOKUP(B30,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G30" s="2">
         <v>29</v>
@@ -23642,20 +23579,20 @@
         <v>30</v>
       </c>
       <c r="B31" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C31" s="4" t="str">
         <f>IF((B31=""),"",VLOOKUP(B31,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>193</v>
+        <v>177</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>370</v>
+        <v>328</v>
       </c>
       <c r="G31" s="2">
         <v>30</v>
@@ -23666,44 +23603,44 @@
         <v>31</v>
       </c>
       <c r="B32" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C32" s="4" t="str">
         <f>IF((B32=""),"",VLOOKUP(B32,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D32" t="s">
-        <v>171</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>172</v>
+        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>193</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>325</v>
+        <v>364</v>
       </c>
       <c r="G32" s="2">
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" s="43" customFormat="1">
       <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
-        <v>13</v>
-      </c>
-      <c r="C33" s="4" t="str">
+      <c r="B33" s="15">
+        <v>14</v>
+      </c>
+      <c r="C33" s="43" t="str">
         <f>IF((B33=""),"",VLOOKUP(B33,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D33" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>326</v>
+        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D33" s="44" t="s">
+        <v>169</v>
+      </c>
+      <c r="E33" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>356</v>
       </c>
       <c r="G33" s="2">
         <v>32</v>
@@ -23714,20 +23651,20 @@
         <v>33</v>
       </c>
       <c r="B34" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C34" s="4" t="str">
         <f>IF((B34=""),"",VLOOKUP(B34,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D34" s="9" t="s">
-        <v>175</v>
+        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>176</v>
+        <v>341</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>329</v>
+        <v>342</v>
       </c>
       <c r="G34" s="2">
         <v>33</v>
@@ -23738,20 +23675,20 @@
         <v>34</v>
       </c>
       <c r="B35" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C35" s="4" t="str">
         <f>IF((B35=""),"",VLOOKUP(B35,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>177</v>
+        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="G35" s="2">
         <v>34</v>
@@ -23762,20 +23699,20 @@
         <v>35</v>
       </c>
       <c r="B36" s="3">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C36" s="4" t="str">
         <f>IF((B36=""),"",VLOOKUP(B36,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D36" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E36" s="26" t="s">
-        <v>193</v>
+        <v>Project is Referred to Minister for Exemption - s.16(2)(b)</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>170</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>369</v>
+        <v>323</v>
       </c>
       <c r="G36" s="2">
         <v>35</v>
@@ -23786,44 +23723,44 @@
         <v>36</v>
       </c>
       <c r="B37" s="3">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C37" s="4" t="str">
         <f>IF((B37=""),"",VLOOKUP(B37,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E37" s="26" t="s">
-        <v>193</v>
+        <v>184</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>364</v>
+        <v>324</v>
       </c>
       <c r="G37" s="2">
         <v>36</v>
       </c>
     </row>
-    <row r="38" spans="1:7" s="43" customFormat="1">
+    <row r="38" spans="1:7">
       <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="15">
-        <v>14</v>
-      </c>
-      <c r="C38" s="43" t="str">
+      <c r="B38" s="3">
+        <v>17</v>
+      </c>
+      <c r="C38" s="4" t="str">
         <f>IF((B38=""),"",VLOOKUP(B38,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
-      </c>
-      <c r="D38" s="44" t="s">
-        <v>169</v>
-      </c>
-      <c r="E38" s="45" t="s">
-        <v>188</v>
-      </c>
-      <c r="F38" s="43" t="s">
-        <v>356</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D38" t="s">
+        <v>171</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G38" s="2">
         <v>37</v>
@@ -23834,20 +23771,20 @@
         <v>38</v>
       </c>
       <c r="B39" s="3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C39" s="4" t="str">
         <f>IF((B39=""),"",VLOOKUP(B39,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>189</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>341</v>
+        <v>174</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="G39" s="2">
         <v>38</v>
@@ -23858,20 +23795,20 @@
         <v>39</v>
       </c>
       <c r="B40" s="3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="C40" s="4" t="str">
         <f>IF((B40=""),"",VLOOKUP(B40,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised DPD - s.16(2)(a)</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>191</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="G40" s="2">
         <v>39</v>
@@ -23882,20 +23819,20 @@
         <v>40</v>
       </c>
       <c r="B41" s="3">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C41" s="4" t="str">
         <f>IF((B41=""),"",VLOOKUP(B41,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project is Referred to Minister for Exemption - s.16(2)(b)</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>169</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>170</v>
+        <v>178</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>323</v>
+        <v>328</v>
       </c>
       <c r="G41" s="2">
         <v>40</v>
@@ -23906,20 +23843,20 @@
         <v>41</v>
       </c>
       <c r="B42" s="3">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C42" s="4" t="str">
         <f>IF((B42=""),"",VLOOKUP(B42,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>184</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D42" t="s">
+        <v>171</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>185</v>
+        <v>172</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="G42" s="2">
         <v>41</v>
@@ -23930,20 +23867,20 @@
         <v>42</v>
       </c>
       <c r="B43" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C43" s="4" t="str">
         <f>IF((B43=""),"",VLOOKUP(B43,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D43" t="s">
-        <v>171</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G43" s="2">
         <v>42</v>
@@ -23954,20 +23891,20 @@
         <v>43</v>
       </c>
       <c r="B44" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C44" s="4" t="str">
         <f>IF((B44=""),"",VLOOKUP(B44,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D44" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G44" s="2">
         <v>43</v>
@@ -23978,20 +23915,20 @@
         <v>44</v>
       </c>
       <c r="B45" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C45" s="4" t="str">
         <f>IF((B45=""),"",VLOOKUP(B45,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="G45" s="2">
         <v>44</v>
@@ -24002,20 +23939,20 @@
         <v>45</v>
       </c>
       <c r="B46" s="3">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C46" s="4" t="str">
         <f>IF((B46=""),"",VLOOKUP(B46,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>178</v>
+        <v>Last Day of Exemption Request: Readiness Decision PHASE</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E46" s="30" t="s">
+        <v>194</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="G46" s="2">
         <v>45</v>
@@ -24026,20 +23963,20 @@
         <v>46</v>
       </c>
       <c r="B47" s="3">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C47" s="4" t="str">
         <f>IF((B47=""),"",VLOOKUP(B47,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E47" s="26" t="s">
-        <v>193</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D47" t="s">
+        <v>171</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>371</v>
+        <v>325</v>
       </c>
       <c r="G47" s="2">
         <v>46</v>
@@ -24050,20 +23987,20 @@
         <v>47</v>
       </c>
       <c r="B48" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C48" s="4" t="str">
         <f>IF((B48=""),"",VLOOKUP(B48,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
-      <c r="D48" t="s">
-        <v>171</v>
+      <c r="D48" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="G48" s="2">
         <v>47</v>
@@ -24074,20 +24011,20 @@
         <v>48</v>
       </c>
       <c r="B49" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C49" s="4" t="str">
         <f>IF((B49=""),"",VLOOKUP(B49,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="G49" s="2">
         <v>48</v>
@@ -24098,20 +24035,20 @@
         <v>49</v>
       </c>
       <c r="B50" s="3">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C50" s="4" t="str">
         <f>IF((B50=""),"",VLOOKUP(B50,Outcomes!$A$2:$D$30,4,FALSE))</f>
         <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G50" s="2">
         <v>49</v>
@@ -24122,20 +24059,20 @@
         <v>50</v>
       </c>
       <c r="B51" s="3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C51" s="4" t="str">
         <f>IF((B51=""),"",VLOOKUP(B51,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D51" s="9" t="s">
-        <v>177</v>
+        <v>Project is Exempt from Requiring an EAC</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>328</v>
+        <v>336</v>
       </c>
       <c r="G51" s="2">
         <v>50</v>
@@ -24146,20 +24083,20 @@
         <v>51</v>
       </c>
       <c r="B52" s="3">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C52" s="4" t="str">
         <f>IF((B52=""),"",VLOOKUP(B52,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D52" s="9" t="s">
-        <v>183</v>
+        <v>Project is Exempt from Requiring an EAC</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>196</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>372</v>
+        <v>337</v>
       </c>
       <c r="G52" s="2">
         <v>51</v>
@@ -24170,20 +24107,20 @@
         <v>52</v>
       </c>
       <c r="B53" s="3">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C53" s="4" t="str">
         <f>IF((B53=""),"",VLOOKUP(B53,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Last Day of Exemption Request: Readiness Decision PHASE</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E53" s="30" t="s">
-        <v>194</v>
+        <v>Refer the Project to the CEAO for Further Decision</v>
+      </c>
+      <c r="D53" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="E53" s="42" t="s">
+        <v>198</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="G53" s="2">
         <v>52</v>
@@ -24194,20 +24131,20 @@
         <v>53</v>
       </c>
       <c r="B54" s="3">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C54" s="4" t="str">
         <f>IF((B54=""),"",VLOOKUP(B54,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D54" t="s">
-        <v>171</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>172</v>
+        <v>Refer the Project to the CEAO for Further Decision</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>199</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="G54" s="2">
         <v>53</v>
@@ -24218,20 +24155,20 @@
         <v>54</v>
       </c>
       <c r="B55" s="3">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C55" s="4" t="str">
         <f>IF((B55=""),"",VLOOKUP(B55,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D55" s="9" t="s">
-        <v>173</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
+      </c>
+      <c r="D55" s="26" t="s">
+        <v>184</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G55" s="2">
         <v>54</v>
@@ -24242,20 +24179,20 @@
         <v>55</v>
       </c>
       <c r="B56" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C56" s="4" t="str">
         <f>IF((B56=""),"",VLOOKUP(B56,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D56" s="9" t="s">
-        <v>175</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D56" t="s">
+        <v>171</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="G56" s="2">
         <v>55</v>
@@ -24266,20 +24203,20 @@
         <v>56</v>
       </c>
       <c r="B57" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C57" s="4" t="str">
         <f>IF((B57=""),"",VLOOKUP(B57,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G57" s="2">
         <v>56</v>
@@ -24290,20 +24227,20 @@
         <v>57</v>
       </c>
       <c r="B58" s="3">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="C58" s="4" t="str">
         <f>IF((B58=""),"",VLOOKUP(B58,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D58" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E58" s="26" t="s">
-        <v>193</v>
+        <v>175</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>373</v>
+        <v>327</v>
       </c>
       <c r="G58" s="2">
         <v>57</v>
@@ -24314,20 +24251,20 @@
         <v>58</v>
       </c>
       <c r="B59" s="3">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C59" s="4" t="str">
         <f>IF((B59=""),"",VLOOKUP(B59,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project is Exempt from Requiring an EAC</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>175</v>
+        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D59" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>195</v>
+        <v>178</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="G59" s="2">
         <v>58</v>
@@ -24338,20 +24275,20 @@
         <v>59</v>
       </c>
       <c r="B60" s="3">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C60" s="4" t="str">
         <f>IF((B60=""),"",VLOOKUP(B60,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project is Exempt from Requiring an EAC</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E60" s="26" t="s">
-        <v>197</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D60" t="s">
+        <v>171</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="G60" s="2">
         <v>59</v>
@@ -24362,20 +24299,20 @@
         <v>60</v>
       </c>
       <c r="B61" s="3">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C61" s="4" t="str">
         <f>IF((B61=""),"",VLOOKUP(B61,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Refer the Project to the CEAO for Further Decision</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>189</v>
-      </c>
-      <c r="E61" s="42" t="s">
-        <v>198</v>
+        <v>173</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>365</v>
+        <v>326</v>
       </c>
       <c r="G61" s="2">
         <v>60</v>
@@ -24386,20 +24323,20 @@
         <v>61</v>
       </c>
       <c r="B62" s="3">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C62" s="4" t="str">
         <f>IF((B62=""),"",VLOOKUP(B62,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Refer the Project to the CEAO for Further Decision</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E62" s="30" t="s">
-        <v>199</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D62" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="G62" s="2">
         <v>61</v>
@@ -24410,20 +24347,20 @@
         <v>62</v>
       </c>
       <c r="B63" s="3">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C63" s="4" t="str">
         <f>IF((B63=""),"",VLOOKUP(B63,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D63" s="26" t="s">
-        <v>184</v>
+        <v>Proponent Withdraws Project from the Exemption Request Process</v>
+      </c>
+      <c r="D63" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="G63" s="2">
         <v>62</v>
@@ -24434,20 +24371,20 @@
         <v>63</v>
       </c>
       <c r="B64" s="3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C64" s="4" t="str">
         <f>IF((B64=""),"",VLOOKUP(B64,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D64" t="s">
-        <v>171</v>
+        <v>CEAO Requires the Proponent to Submit a Revised Exemption Request DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>189</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F64" s="1" t="s">
-        <v>325</v>
+        <v>341</v>
+      </c>
+      <c r="F64" s="42" t="s">
+        <v>342</v>
       </c>
       <c r="G64" s="2">
         <v>63</v>
@@ -24458,20 +24395,20 @@
         <v>64</v>
       </c>
       <c r="B65" s="3">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C65" s="4" t="str">
         <f>IF((B65=""),"",VLOOKUP(B65,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D65" s="9" t="s">
-        <v>173</v>
+        <v>CEAO Requires the Proponent to Submit a Revised Exemption Request DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>191</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>326</v>
+        <v>192</v>
+      </c>
+      <c r="F65" s="41" t="s">
+        <v>343</v>
       </c>
       <c r="G65" s="2">
         <v>64</v>
@@ -24482,20 +24419,20 @@
         <v>65</v>
       </c>
       <c r="B66" s="3">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C66" s="4" t="str">
         <f>IF((B66=""),"",VLOOKUP(B66,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D66" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E66" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>327</v>
+        <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E66" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="F66" s="30" t="s">
+        <v>348</v>
       </c>
       <c r="G66" s="2">
         <v>65</v>
@@ -24506,20 +24443,20 @@
         <v>66</v>
       </c>
       <c r="B67" s="3">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C67" s="4" t="str">
         <f>IF((B67=""),"",VLOOKUP(B67,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D67" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E67" s="1" t="s">
-        <v>178</v>
+        <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E67" s="42" t="s">
+        <v>190</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="G67" s="2">
         <v>66</v>
@@ -24530,44 +24467,44 @@
         <v>67</v>
       </c>
       <c r="B68" s="3">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C68" s="4" t="str">
         <f>IF((B68=""),"",VLOOKUP(B68,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Exemption Request is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D68" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E68" s="26" t="s">
-        <v>193</v>
+        <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>375</v>
+        <v>343</v>
       </c>
       <c r="G68" s="2">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="1:7">
+    <row r="69" spans="1:7" s="37" customFormat="1">
       <c r="A69" s="2">
         <v>68</v>
       </c>
       <c r="B69" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C69" s="4" t="str">
         <f>IF((B69=""),"",VLOOKUP(B69,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D69" t="s">
-        <v>171</v>
+        <v>Project Moves to EAC Assessment: Process Planning PHASE - s.18(1)(a)</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>182</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>325</v>
+        <v>352</v>
       </c>
       <c r="G69" s="2">
         <v>68</v>
@@ -24578,20 +24515,20 @@
         <v>69</v>
       </c>
       <c r="B70" s="3">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C70" s="4" t="str">
         <f>IF((B70=""),"",VLOOKUP(B70,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D70" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>174</v>
+        <v>Project Moves to EAC Assessment: Process Planning PHASE - s.18(1)(a)</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="E70" s="26" t="s">
+        <v>200</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>326</v>
+        <v>349</v>
       </c>
       <c r="G70" s="2">
         <v>69</v>
@@ -24602,20 +24539,20 @@
         <v>70</v>
       </c>
       <c r="B71" s="3">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C71" s="4" t="str">
         <f>IF((B71=""),"",VLOOKUP(B71,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D71" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>176</v>
+        <v>Project is Referred to Minister for EAC Assessment: Process Planning - s.18(1)(b)</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" s="26" t="s">
+        <v>202</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G71" s="2">
         <v>70</v>
@@ -24626,20 +24563,20 @@
         <v>71</v>
       </c>
       <c r="B72" s="3">
-        <v>25</v>
+        <v>36</v>
       </c>
       <c r="C72" s="4" t="str">
-        <f>IF((B72=""),"",VLOOKUP(B72,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D72" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>178</v>
+        <f>IF((B72=""),"",VLOOKUP(B72,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>No Federal Involvement triggered for this WORK</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E72" s="30" t="s">
+        <v>319</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="G72" s="2">
         <v>71</v>
@@ -24650,20 +24587,20 @@
         <v>72</v>
       </c>
       <c r="B73" s="3">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C73" s="4" t="str">
-        <f>IF((B73=""),"",VLOOKUP(B73,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the Exemption Request Process</v>
-      </c>
-      <c r="D73" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E73" s="26" t="s">
-        <v>193</v>
+        <f>IF((B73=""),"",VLOOKUP(B73,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>Federal Substitution Request Approved</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E73" s="30" t="s">
+        <v>321</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>374</v>
+        <v>322</v>
       </c>
       <c r="G73" s="2">
         <v>72</v>
@@ -24674,20 +24611,20 @@
         <v>73</v>
       </c>
       <c r="B74" s="3">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C74" s="4" t="str">
-        <f>IF((B74=""),"",VLOOKUP(B74,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised Exemption Request DPD - s.16(2)(a)</v>
+        <f>IF((B74=""),"",VLOOKUP(B74,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>Other form of Federal Involvement (Coordination, etc.)</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="F74" s="42" t="s">
-        <v>342</v>
+        <v>169</v>
+      </c>
+      <c r="E74" s="30" t="s">
+        <v>202</v>
+      </c>
+      <c r="F74" s="1" t="s">
+        <v>323</v>
       </c>
       <c r="G74" s="2">
         <v>73</v>
@@ -24698,20 +24635,20 @@
         <v>74</v>
       </c>
       <c r="B75" s="3">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="C75" s="4" t="str">
-        <f>IF((B75=""),"",VLOOKUP(B75,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised Exemption Request DPD - s.16(2)(a)</v>
+        <f>IF((B75=""),"",VLOOKUP(B75,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>A Matter has been Referred for Dispute Resolution</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="F75" s="41" t="s">
-        <v>343</v>
+        <v>185</v>
+      </c>
+      <c r="F75" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="G75" s="2">
         <v>74</v>
@@ -24722,20 +24659,20 @@
         <v>75</v>
       </c>
       <c r="B76" s="3">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C76" s="4" t="str">
-        <f>IF((B76=""),"",VLOOKUP(B76,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E76" s="30" t="s">
-        <v>347</v>
-      </c>
-      <c r="F76" s="30" t="s">
-        <v>348</v>
+        <f>IF((B76=""),"",VLOOKUP(B76,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D76" t="s">
+        <v>171</v>
+      </c>
+      <c r="E76" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F76" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G76" s="2">
         <v>75</v>
@@ -24746,20 +24683,20 @@
         <v>76</v>
       </c>
       <c r="B77" s="3">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C77" s="4" t="str">
-        <f>IF((B77=""),"",VLOOKUP(B77,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E77" s="42" t="s">
-        <v>190</v>
+        <f>IF((B77=""),"",VLOOKUP(B77,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D77" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>346</v>
+        <v>326</v>
       </c>
       <c r="G77" s="2">
         <v>76</v>
@@ -24770,44 +24707,44 @@
         <v>77</v>
       </c>
       <c r="B78" s="3">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C78" s="4" t="str">
-        <f>IF((B78=""),"",VLOOKUP(B78,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>CEAO Requires the Proponent to Submit a Revised EAC Assessment DPD - s.16(2)(a)</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>191</v>
+        <f>IF((B78=""),"",VLOOKUP(B78,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D78" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="G78" s="2">
         <v>77</v>
       </c>
     </row>
-    <row r="79" spans="1:7" s="37" customFormat="1">
+    <row r="79" spans="1:7">
       <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="B79" s="3">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="C79" s="4" t="str">
-        <f>IF((B79=""),"",VLOOKUP(B79,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project Moves to EAC Assessment: Process Planning PHASE - s.18(1)(a)</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>182</v>
+        <f>IF((B79=""),"",VLOOKUP(B79,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D79" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>201</v>
+        <v>178</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>352</v>
+        <v>328</v>
       </c>
       <c r="G79" s="2">
         <v>78</v>
@@ -24818,20 +24755,20 @@
         <v>79</v>
       </c>
       <c r="B80" s="3">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C80" s="4" t="str">
-        <f>IF((B80=""),"",VLOOKUP(B80,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project Moves to EAC Assessment: Process Planning PHASE - s.18(1)(a)</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="E80" s="26" t="s">
-        <v>200</v>
+        <f>IF((B80=""),"",VLOOKUP(B80,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+      </c>
+      <c r="D80" t="s">
+        <v>171</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>349</v>
+        <v>325</v>
       </c>
       <c r="G80" s="2">
         <v>79</v>
@@ -24842,20 +24779,20 @@
         <v>80</v>
       </c>
       <c r="B81" s="3">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C81" s="4" t="str">
-        <f>IF((B81=""),"",VLOOKUP(B81,Outcomes!$A$2:$D$30,4,FALSE))</f>
-        <v>Project is Referred to Minister for EAC Assessment: Process Planning - s.18(1)(b)</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E81" s="26" t="s">
-        <v>202</v>
+        <f>IF((B81=""),"",VLOOKUP(B81,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+      </c>
+      <c r="D81" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="E81" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G81" s="2">
         <v>80</v>
@@ -24866,20 +24803,20 @@
         <v>81</v>
       </c>
       <c r="B82" s="3">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C82" s="4" t="str">
         <f>IF((B82=""),"",VLOOKUP(B82,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>No Federal Involvement triggered for this WORK</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E82" s="30" t="s">
-        <v>319</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+      </c>
+      <c r="D82" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
       <c r="G82" s="2">
         <v>81</v>
@@ -24890,20 +24827,20 @@
         <v>82</v>
       </c>
       <c r="B83" s="3">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C83" s="4" t="str">
         <f>IF((B83=""),"",VLOOKUP(B83,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Federal Substitution Request Approved</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E83" s="30" t="s">
-        <v>321</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+      </c>
+      <c r="D83" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>322</v>
+        <v>328</v>
       </c>
       <c r="G83" s="2">
         <v>82</v>
@@ -24914,20 +24851,20 @@
         <v>83</v>
       </c>
       <c r="B84" s="3">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C84" s="4" t="str">
         <f>IF((B84=""),"",VLOOKUP(B84,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Other form of Federal Involvement (Coordination, etc.)</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>169</v>
+        <v>Last Day of EAC Assessment: Process Planning PHASE</v>
+      </c>
+      <c r="D84" s="9" t="s">
+        <v>191</v>
       </c>
       <c r="E84" s="30" t="s">
-        <v>202</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>323</v>
+        <v>330</v>
+      </c>
+      <c r="F84" s="42" t="s">
+        <v>358</v>
       </c>
       <c r="G84" s="2">
         <v>83</v>
@@ -24938,20 +24875,20 @@
         <v>84</v>
       </c>
       <c r="B85" s="3">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C85" s="4" t="str">
         <f>IF((B85=""),"",VLOOKUP(B85,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
+        <v>EAO's Viewpoint is POSITIVE</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>184</v>
+        <v>169</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>185</v>
+        <v>170</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="G85" s="2">
         <v>84</v>
@@ -24962,20 +24899,20 @@
         <v>85</v>
       </c>
       <c r="B86" s="3">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C86" s="4" t="str">
         <f>IF((B86=""),"",VLOOKUP(B86,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D86" t="s">
-        <v>171</v>
+        <v>EAO's Viewpoint is NEGATIVE</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G86" s="2">
         <v>85</v>
@@ -24986,20 +24923,20 @@
         <v>86</v>
       </c>
       <c r="B87" s="3">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C87" s="4" t="str">
         <f>IF((B87=""),"",VLOOKUP(B87,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D87" s="9" t="s">
-        <v>173</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>174</v>
+        <v>185</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="G87" s="2">
         <v>86</v>
@@ -25010,20 +24947,20 @@
         <v>87</v>
       </c>
       <c r="B88" s="3">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C88" s="4" t="str">
         <f>IF((B88=""),"",VLOOKUP(B88,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
-      <c r="D88" s="9" t="s">
-        <v>175</v>
+      <c r="D88" t="s">
+        <v>171</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G88" s="2">
         <v>87</v>
@@ -25034,20 +24971,20 @@
         <v>88</v>
       </c>
       <c r="B89" s="3">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C89" s="4" t="str">
         <f>IF((B89=""),"",VLOOKUP(B89,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D89" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G89" s="2">
         <v>88</v>
@@ -25058,20 +24995,20 @@
         <v>89</v>
       </c>
       <c r="B90" s="3">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C90" s="4" t="str">
         <f>IF((B90=""),"",VLOOKUP(B90,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D90" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E90" s="26" t="s">
-        <v>193</v>
+        <v>175</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>186</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>376</v>
+        <v>327</v>
       </c>
       <c r="G90" s="2">
         <v>89</v>
@@ -25082,20 +25019,20 @@
         <v>90</v>
       </c>
       <c r="B91" s="3">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C91" s="4" t="str">
         <f>IF((B91=""),"",VLOOKUP(B91,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D91" t="s">
-        <v>171</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D91" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G91" s="2">
         <v>90</v>
@@ -25106,20 +25043,20 @@
         <v>91</v>
       </c>
       <c r="B92" s="3">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C92" s="4" t="str">
         <f>IF((B92=""),"",VLOOKUP(B92,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
-      <c r="D92" s="9" t="s">
-        <v>173</v>
+      <c r="D92" t="s">
+        <v>171</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G92" s="2">
         <v>91</v>
@@ -25130,20 +25067,20 @@
         <v>92</v>
       </c>
       <c r="B93" s="3">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C93" s="4" t="str">
         <f>IF((B93=""),"",VLOOKUP(B93,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D93" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="G93" s="2">
         <v>92</v>
@@ -25154,20 +25091,20 @@
         <v>93</v>
       </c>
       <c r="B94" s="3">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C94" s="4" t="str">
         <f>IF((B94=""),"",VLOOKUP(B94,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D94" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G94" s="2">
         <v>93</v>
@@ -25178,20 +25115,20 @@
         <v>94</v>
       </c>
       <c r="B95" s="3">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C95" s="4" t="str">
         <f>IF((B95=""),"",VLOOKUP(B95,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D95" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E95" s="26" t="s">
-        <v>193</v>
+        <v>177</v>
+      </c>
+      <c r="E95" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>377</v>
+        <v>328</v>
       </c>
       <c r="G95" s="2">
         <v>94</v>
@@ -25202,20 +25139,20 @@
         <v>95</v>
       </c>
       <c r="B96" s="3">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C96" s="4" t="str">
         <f>IF((B96=""),"",VLOOKUP(B96,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Last Day of EAC Assessment: Process Planning PHASE</v>
-      </c>
-      <c r="D96" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E96" s="30" t="s">
-        <v>330</v>
-      </c>
-      <c r="F96" s="42" t="s">
-        <v>358</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E96" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="F96" s="1" t="s">
+        <v>324</v>
       </c>
       <c r="G96" s="2">
         <v>95</v>
@@ -25226,20 +25163,20 @@
         <v>96</v>
       </c>
       <c r="B97" s="3">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="C97" s="4" t="str">
         <f>IF((B97=""),"",VLOOKUP(B97,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAO's Viewpoint is POSITIVE</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>169</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D97" t="s">
+        <v>171</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G97" s="2">
         <v>96</v>
@@ -25250,20 +25187,20 @@
         <v>97</v>
       </c>
       <c r="B98" s="3">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C98" s="4" t="str">
         <f>IF((B98=""),"",VLOOKUP(B98,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAO's Viewpoint is NEGATIVE</v>
-      </c>
-      <c r="D98" s="1" t="s">
-        <v>169</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D98" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G98" s="2">
         <v>97</v>
@@ -25274,20 +25211,20 @@
         <v>98</v>
       </c>
       <c r="B99" s="3">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C99" s="4" t="str">
         <f>IF((B99=""),"",VLOOKUP(B99,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D99" s="1" t="s">
-        <v>184</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D99" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="G99" s="2">
         <v>98</v>
@@ -25298,20 +25235,20 @@
         <v>99</v>
       </c>
       <c r="B100" s="3">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C100" s="4" t="str">
         <f>IF((B100=""),"",VLOOKUP(B100,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
-      <c r="D100" t="s">
-        <v>171</v>
+      <c r="D100" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G100" s="2">
         <v>99</v>
@@ -25322,20 +25259,20 @@
         <v>100</v>
       </c>
       <c r="B101" s="3">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C101" s="4" t="str">
         <f>IF((B101=""),"",VLOOKUP(B101,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D101" s="9" t="s">
-        <v>173</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+      </c>
+      <c r="D101" t="s">
+        <v>171</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G101" s="2">
         <v>100</v>
@@ -25346,20 +25283,20 @@
         <v>101</v>
       </c>
       <c r="B102" s="3">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C102" s="4" t="str">
         <f>IF((B102=""),"",VLOOKUP(B102,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D102" s="9" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="G102" s="2">
         <v>101</v>
@@ -25370,20 +25307,20 @@
         <v>102</v>
       </c>
       <c r="B103" s="3">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C103" s="4" t="str">
         <f>IF((B103=""),"",VLOOKUP(B103,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D103" s="9" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="G103" s="2">
         <v>102</v>
@@ -25394,20 +25331,20 @@
         <v>103</v>
       </c>
       <c r="B104" s="3">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C104" s="4" t="str">
         <f>IF((B104=""),"",VLOOKUP(B104,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D104" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E104" s="26" t="s">
-        <v>193</v>
+        <v>177</v>
+      </c>
+      <c r="E104" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>379</v>
+        <v>328</v>
       </c>
       <c r="G104" s="2">
         <v>103</v>
@@ -25418,20 +25355,20 @@
         <v>104</v>
       </c>
       <c r="B105" s="3">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C105" s="4" t="str">
         <f>IF((B105=""),"",VLOOKUP(B105,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D105" t="s">
-        <v>171</v>
-      </c>
-      <c r="E105" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F105" s="1" t="s">
-        <v>325</v>
+        <v>Last Day of EAC Assessment: EAC Application Review PHASE</v>
+      </c>
+      <c r="D105" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="E105" s="30" t="s">
+        <v>331</v>
+      </c>
+      <c r="F105" s="42" t="s">
+        <v>359</v>
       </c>
       <c r="G105" s="2">
         <v>104</v>
@@ -25442,20 +25379,20 @@
         <v>105</v>
       </c>
       <c r="B106" s="3">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="C106" s="4" t="str">
         <f>IF((B106=""),"",VLOOKUP(B106,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D106" s="9" t="s">
-        <v>173</v>
+        <v>EAO's Viewpoint is POSITIVE</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="G106" s="2">
         <v>105</v>
@@ -25466,20 +25403,20 @@
         <v>106</v>
       </c>
       <c r="B107" s="3">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C107" s="4" t="str">
         <f>IF((B107=""),"",VLOOKUP(B107,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D107" s="9" t="s">
-        <v>175</v>
+        <v>EAO's Viewpoint is NEGATIVE</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="G107" s="2">
         <v>106</v>
@@ -25490,20 +25427,20 @@
         <v>107</v>
       </c>
       <c r="B108" s="3">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C108" s="4" t="str">
         <f>IF((B108=""),"",VLOOKUP(B108,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D108" s="9" t="s">
-        <v>177</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>184</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="G108" s="2">
         <v>107</v>
@@ -25514,20 +25451,20 @@
         <v>108</v>
       </c>
       <c r="B109" s="3">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C109" s="4" t="str">
         <f>IF((B109=""),"",VLOOKUP(B109,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D109" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E109" s="26" t="s">
-        <v>193</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D109" t="s">
+        <v>171</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>172</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>378</v>
+        <v>325</v>
       </c>
       <c r="G109" s="2">
         <v>108</v>
@@ -25538,20 +25475,20 @@
         <v>109</v>
       </c>
       <c r="B110" s="3">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C110" s="4" t="str">
         <f>IF((B110=""),"",VLOOKUP(B110,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D110" s="1" t="s">
-        <v>184</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D110" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="G110" s="2">
         <v>109</v>
@@ -25562,20 +25499,20 @@
         <v>110</v>
       </c>
       <c r="B111" s="3">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C111" s="4" t="str">
         <f>IF((B111=""),"",VLOOKUP(B111,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
-      <c r="D111" t="s">
-        <v>171</v>
+      <c r="D111" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E111" s="1" t="s">
-        <v>172</v>
+        <v>186</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="G111" s="2">
         <v>110</v>
@@ -25586,20 +25523,20 @@
         <v>111</v>
       </c>
       <c r="B112" s="3">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="C112" s="4" t="str">
         <f>IF((B112=""),"",VLOOKUP(B112,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E112" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="G112" s="2">
         <v>111</v>
@@ -25610,20 +25547,20 @@
         <v>112</v>
       </c>
       <c r="B113" s="3">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C113" s="4" t="str">
         <f>IF((B113=""),"",VLOOKUP(B113,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D113" s="9" t="s">
-        <v>175</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+      </c>
+      <c r="D113" t="s">
+        <v>171</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G113" s="2">
         <v>112</v>
@@ -25634,20 +25571,20 @@
         <v>113</v>
       </c>
       <c r="B114" s="3">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C114" s="4" t="str">
         <f>IF((B114=""),"",VLOOKUP(B114,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D114" s="9" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="G114" s="2">
         <v>113</v>
@@ -25658,20 +25595,20 @@
         <v>114</v>
       </c>
       <c r="B115" s="3">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="C115" s="4" t="str">
         <f>IF((B115=""),"",VLOOKUP(B115,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D115" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E115" s="26" t="s">
-        <v>193</v>
+        <v>175</v>
+      </c>
+      <c r="E115" s="1" t="s">
+        <v>176</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>380</v>
+        <v>329</v>
       </c>
       <c r="G115" s="2">
         <v>114</v>
@@ -25682,20 +25619,20 @@
         <v>115</v>
       </c>
       <c r="B116" s="3">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="C116" s="4" t="str">
         <f>IF((B116=""),"",VLOOKUP(B116,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
         <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
-      <c r="D116" t="s">
-        <v>171</v>
+      <c r="D116" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="G116" s="2">
         <v>115</v>
@@ -25706,20 +25643,20 @@
         <v>116</v>
       </c>
       <c r="B117" s="3">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C117" s="4" t="str">
         <f>IF((B117=""),"",VLOOKUP(B117,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D117" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E117" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F117" s="1" t="s">
-        <v>326</v>
+        <v>Revised EAC Application Sufficient to Proceed</v>
+      </c>
+      <c r="D117" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E117" s="30" t="s">
+        <v>332</v>
+      </c>
+      <c r="F117" s="42" t="s">
+        <v>360</v>
       </c>
       <c r="G117" s="2">
         <v>116</v>
@@ -25730,20 +25667,20 @@
         <v>117</v>
       </c>
       <c r="B118" s="3">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C118" s="4" t="str">
         <f>IF((B118=""),"",VLOOKUP(B118,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
+        <v>Proponent must provide an updated Revised EAC Application</v>
       </c>
       <c r="D118" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E118" s="1" t="s">
-        <v>176</v>
+        <v>182</v>
+      </c>
+      <c r="E118" s="30" t="s">
+        <v>333</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>329</v>
+        <v>361</v>
       </c>
       <c r="G118" s="2">
         <v>117</v>
@@ -25754,20 +25691,20 @@
         <v>118</v>
       </c>
       <c r="B119" s="3">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="C119" s="4" t="str">
         <f>IF((B119=""),"",VLOOKUP(B119,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D119" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E119" s="1" t="s">
-        <v>178</v>
+        <v>Proponent must provide an updated Revised EAC Application</v>
+      </c>
+      <c r="D119" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="E119" s="30" t="s">
+        <v>334</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>328</v>
+        <v>362</v>
       </c>
       <c r="G119" s="2">
         <v>118</v>
@@ -25778,20 +25715,20 @@
         <v>119</v>
       </c>
       <c r="B120" s="3">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="C120" s="4" t="str">
         <f>IF((B120=""),"",VLOOKUP(B120,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D120" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E120" s="26" t="s">
-        <v>193</v>
+        <v>A Matter has been Referred for Dispute Resolution</v>
+      </c>
+      <c r="D120" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="E120" s="1" t="s">
+        <v>185</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>381</v>
+        <v>324</v>
       </c>
       <c r="G120" s="2">
         <v>119</v>
@@ -25802,20 +25739,20 @@
         <v>120</v>
       </c>
       <c r="B121" s="3">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="C121" s="4" t="str">
         <f>IF((B121=""),"",VLOOKUP(B121,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Last Day of EAC Assessment: EAC Application Review PHASE</v>
-      </c>
-      <c r="D121" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="E121" s="30" t="s">
-        <v>331</v>
-      </c>
-      <c r="F121" s="42" t="s">
-        <v>359</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D121" t="s">
+        <v>171</v>
+      </c>
+      <c r="E121" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="F121" s="1" t="s">
+        <v>325</v>
       </c>
       <c r="G121" s="2">
         <v>120</v>
@@ -25826,20 +25763,20 @@
         <v>121</v>
       </c>
       <c r="B122" s="3">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C122" s="4" t="str">
         <f>IF((B122=""),"",VLOOKUP(B122,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAO's Viewpoint is POSITIVE</v>
-      </c>
-      <c r="D122" s="1" t="s">
-        <v>169</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>173</v>
       </c>
       <c r="E122" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G122" s="2">
         <v>121</v>
@@ -25850,20 +25787,20 @@
         <v>122</v>
       </c>
       <c r="B123" s="3">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="C123" s="4" t="str">
         <f>IF((B123=""),"",VLOOKUP(B123,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAO's Viewpoint is NEGATIVE</v>
-      </c>
-      <c r="D123" s="1" t="s">
-        <v>169</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D123" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="E123" s="1" t="s">
-        <v>170</v>
+        <v>186</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="G123" s="2">
         <v>122</v>
@@ -25874,20 +25811,20 @@
         <v>123</v>
       </c>
       <c r="B124" s="3">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C124" s="4" t="str">
         <f>IF((B124=""),"",VLOOKUP(B124,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D124" s="1" t="s">
-        <v>184</v>
+        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+      </c>
+      <c r="D124" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="G124" s="2">
         <v>123</v>
@@ -25898,11 +25835,11 @@
         <v>124</v>
       </c>
       <c r="B125" s="3">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C125" s="4" t="str">
         <f>IF((B125=""),"",VLOOKUP(B125,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D125" t="s">
         <v>171</v>
@@ -25922,11 +25859,11 @@
         <v>125</v>
       </c>
       <c r="B126" s="3">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C126" s="4" t="str">
         <f>IF((B126=""),"",VLOOKUP(B126,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D126" s="9" t="s">
         <v>173</v>
@@ -25946,20 +25883,20 @@
         <v>126</v>
       </c>
       <c r="B127" s="3">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C127" s="4" t="str">
         <f>IF((B127=""),"",VLOOKUP(B127,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D127" s="9" t="s">
         <v>175</v>
       </c>
       <c r="E127" s="1" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G127" s="2">
         <v>126</v>
@@ -25970,11 +25907,11 @@
         <v>127</v>
       </c>
       <c r="B128" s="3">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C128" s="4" t="str">
         <f>IF((B128=""),"",VLOOKUP(B128,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
+        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
       </c>
       <c r="D128" s="9" t="s">
         <v>177</v>
@@ -25994,20 +25931,20 @@
         <v>128</v>
       </c>
       <c r="B129" s="3">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="C129" s="4" t="str">
         <f>IF((B129=""),"",VLOOKUP(B129,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D129" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E129" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="F129" s="1" t="s">
-        <v>382</v>
+        <v>Last Day of EAC Assessment: Effects Assessment PHASE</v>
+      </c>
+      <c r="D129" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E129" s="30" t="s">
+        <v>335</v>
+      </c>
+      <c r="F129" s="42" t="s">
+        <v>363</v>
       </c>
       <c r="G129" s="2">
         <v>128</v>
@@ -26018,7 +25955,7 @@
         <v>129</v>
       </c>
       <c r="B130" s="3">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C130" s="4" t="str">
         <f>IF((B130=""),"",VLOOKUP(B130,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
@@ -26042,7 +25979,7 @@
         <v>130</v>
       </c>
       <c r="B131" s="3">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C131" s="4" t="str">
         <f>IF((B131=""),"",VLOOKUP(B131,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
@@ -26066,7 +26003,7 @@
         <v>131</v>
       </c>
       <c r="B132" s="3">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C132" s="4" t="str">
         <f>IF((B132=""),"",VLOOKUP(B132,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
@@ -26090,7 +26027,7 @@
         <v>132</v>
       </c>
       <c r="B133" s="3">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="C133" s="4" t="str">
         <f>IF((B133=""),"",VLOOKUP(B133,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
@@ -26114,20 +26051,20 @@
         <v>133</v>
       </c>
       <c r="B134" s="3">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C134" s="4" t="str">
         <f>IF((B134=""),"",VLOOKUP(B134,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D134" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E134" s="26" t="s">
-        <v>193</v>
+        <v>Environmental Assessment Certificate GRANTED</v>
+      </c>
+      <c r="D134" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>195</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>383</v>
+        <v>336</v>
       </c>
       <c r="G134" s="2">
         <v>133</v>
@@ -26138,20 +26075,20 @@
         <v>134</v>
       </c>
       <c r="B135" s="3">
-        <v>57</v>
+        <v>64</v>
       </c>
       <c r="C135" s="4" t="str">
         <f>IF((B135=""),"",VLOOKUP(B135,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Revised EAC Application Sufficient to Proceed</v>
+        <v>Environmental Assessment Certificate GRANTED</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>191</v>
+        <v>196</v>
       </c>
       <c r="E135" s="30" t="s">
-        <v>332</v>
-      </c>
-      <c r="F135" s="42" t="s">
-        <v>360</v>
+        <v>197</v>
+      </c>
+      <c r="F135" s="1" t="s">
+        <v>337</v>
       </c>
       <c r="G135" s="2">
         <v>134</v>
@@ -26162,20 +26099,20 @@
         <v>135</v>
       </c>
       <c r="B136" s="3">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C136" s="4" t="str">
         <f>IF((B136=""),"",VLOOKUP(B136,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent must provide an updated Revised EAC Application</v>
+        <v>Environmental Assessment Certificate REFUSED</v>
       </c>
       <c r="D136" s="9" t="s">
-        <v>182</v>
-      </c>
-      <c r="E136" s="30" t="s">
-        <v>333</v>
+        <v>175</v>
+      </c>
+      <c r="E136" s="9" t="s">
+        <v>195</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>361</v>
+        <v>336</v>
       </c>
       <c r="G136" s="2">
         <v>135</v>
@@ -26186,531 +26123,27 @@
         <v>136</v>
       </c>
       <c r="B137" s="3">
-        <v>58</v>
+        <v>65</v>
       </c>
       <c r="C137" s="4" t="str">
         <f>IF((B137=""),"",VLOOKUP(B137,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent must provide an updated Revised EAC Application</v>
-      </c>
-      <c r="D137" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="E137" s="30" t="s">
-        <v>334</v>
+        <v>Environmental Assessment Certificate REFUSED</v>
+      </c>
+      <c r="D137" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="E137" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>362</v>
+        <v>328</v>
       </c>
       <c r="G137" s="2">
         <v>136</v>
       </c>
     </row>
-    <row r="138" spans="1:7">
-      <c r="A138" s="2">
-        <v>137</v>
-      </c>
-      <c r="B138" s="3">
-        <v>59</v>
-      </c>
-      <c r="C138" s="4" t="str">
-        <f>IF((B138=""),"",VLOOKUP(B138,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>A Matter has been Referred for Dispute Resolution</v>
-      </c>
-      <c r="D138" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E138" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="F138" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="G138" s="2">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="139" spans="1:7">
-      <c r="A139" s="2">
-        <v>138</v>
-      </c>
-      <c r="B139" s="3">
-        <v>60</v>
-      </c>
-      <c r="C139" s="4" t="str">
-        <f>IF((B139=""),"",VLOOKUP(B139,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D139" t="s">
-        <v>171</v>
-      </c>
-      <c r="E139" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F139" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G139" s="2">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="140" spans="1:7">
-      <c r="A140" s="2">
-        <v>139</v>
-      </c>
-      <c r="B140" s="3">
-        <v>60</v>
-      </c>
-      <c r="C140" s="4" t="str">
-        <f>IF((B140=""),"",VLOOKUP(B140,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D140" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E140" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F140" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G140" s="2">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="141" spans="1:7">
-      <c r="A141" s="2">
-        <v>140</v>
-      </c>
-      <c r="B141" s="3">
-        <v>60</v>
-      </c>
-      <c r="C141" s="4" t="str">
-        <f>IF((B141=""),"",VLOOKUP(B141,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D141" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E141" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="F141" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="G141" s="2">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="142" spans="1:7">
-      <c r="A142" s="2">
-        <v>141</v>
-      </c>
-      <c r="B142" s="3">
-        <v>60</v>
-      </c>
-      <c r="C142" s="4" t="str">
-        <f>IF((B142=""),"",VLOOKUP(B142,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D142" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E142" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F142" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G142" s="2">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="143" spans="1:7">
-      <c r="A143" s="2">
-        <v>142</v>
-      </c>
-      <c r="B143" s="3">
-        <v>60</v>
-      </c>
-      <c r="C143" s="4" t="str">
-        <f>IF((B143=""),"",VLOOKUP(B143,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>EAC Assessment is Terminated under s.39(d) of EA Act (2018)</v>
-      </c>
-      <c r="D143" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E143" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="F143" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="G143" s="2">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="144" spans="1:7">
-      <c r="A144" s="2">
-        <v>143</v>
-      </c>
-      <c r="B144" s="3">
-        <v>61</v>
-      </c>
-      <c r="C144" s="4" t="str">
-        <f>IF((B144=""),"",VLOOKUP(B144,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D144" t="s">
-        <v>171</v>
-      </c>
-      <c r="E144" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F144" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G144" s="2">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="145" spans="1:7">
-      <c r="A145" s="2">
-        <v>144</v>
-      </c>
-      <c r="B145" s="3">
-        <v>61</v>
-      </c>
-      <c r="C145" s="4" t="str">
-        <f>IF((B145=""),"",VLOOKUP(B145,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D145" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E145" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F145" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G145" s="2">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="146" spans="1:7">
-      <c r="A146" s="2">
-        <v>145</v>
-      </c>
-      <c r="B146" s="3">
-        <v>61</v>
-      </c>
-      <c r="C146" s="4" t="str">
-        <f>IF((B146=""),"",VLOOKUP(B146,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D146" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E146" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F146" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="G146" s="2">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="147" spans="1:7">
-      <c r="A147" s="2">
-        <v>146</v>
-      </c>
-      <c r="B147" s="3">
-        <v>61</v>
-      </c>
-      <c r="C147" s="4" t="str">
-        <f>IF((B147=""),"",VLOOKUP(B147,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D147" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E147" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F147" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G147" s="2">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="148" spans="1:7">
-      <c r="A148" s="2">
-        <v>147</v>
-      </c>
-      <c r="B148" s="3">
-        <v>61</v>
-      </c>
-      <c r="C148" s="4" t="str">
-        <f>IF((B148=""),"",VLOOKUP(B148,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D148" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E148" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="F148" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="G148" s="2">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="149" spans="1:7">
-      <c r="A149" s="2">
-        <v>148</v>
-      </c>
-      <c r="B149" s="3">
-        <v>62</v>
-      </c>
-      <c r="C149" s="4" t="str">
-        <f>IF((B149=""),"",VLOOKUP(B149,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Last Day of EAC Assessment: Effects Assessment PHASE</v>
-      </c>
-      <c r="D149" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="E149" s="30" t="s">
-        <v>335</v>
-      </c>
-      <c r="F149" s="42" t="s">
-        <v>363</v>
-      </c>
-      <c r="G149" s="2">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="150" spans="1:7">
-      <c r="A150" s="2">
-        <v>149</v>
-      </c>
-      <c r="B150" s="3">
-        <v>63</v>
-      </c>
-      <c r="C150" s="4" t="str">
-        <f>IF((B150=""),"",VLOOKUP(B150,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D150" t="s">
-        <v>171</v>
-      </c>
-      <c r="E150" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="F150" s="1" t="s">
-        <v>325</v>
-      </c>
-      <c r="G150" s="2">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="151" spans="1:7">
-      <c r="A151" s="2">
-        <v>150</v>
-      </c>
-      <c r="B151" s="3">
-        <v>63</v>
-      </c>
-      <c r="C151" s="4" t="str">
-        <f>IF((B151=""),"",VLOOKUP(B151,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D151" s="9" t="s">
-        <v>173</v>
-      </c>
-      <c r="E151" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="F151" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G151" s="2">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7">
-      <c r="A152" s="2">
-        <v>151</v>
-      </c>
-      <c r="B152" s="3">
-        <v>63</v>
-      </c>
-      <c r="C152" s="4" t="str">
-        <f>IF((B152=""),"",VLOOKUP(B152,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D152" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E152" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="F152" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="G152" s="2">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7">
-      <c r="A153" s="2">
-        <v>152</v>
-      </c>
-      <c r="B153" s="3">
-        <v>63</v>
-      </c>
-      <c r="C153" s="4" t="str">
-        <f>IF((B153=""),"",VLOOKUP(B153,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D153" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E153" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F153" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G153" s="2">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7">
-      <c r="A154" s="2">
-        <v>153</v>
-      </c>
-      <c r="B154" s="3">
-        <v>63</v>
-      </c>
-      <c r="C154" s="4" t="str">
-        <f>IF((B154=""),"",VLOOKUP(B154,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Proponent Withdraws Project from the EAC Assessment Process</v>
-      </c>
-      <c r="D154" s="9" t="s">
-        <v>183</v>
-      </c>
-      <c r="E154" s="26" t="s">
-        <v>193</v>
-      </c>
-      <c r="F154" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="G154" s="2">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7">
-      <c r="A155" s="2">
-        <v>154</v>
-      </c>
-      <c r="B155" s="3">
-        <v>64</v>
-      </c>
-      <c r="C155" s="4" t="str">
-        <f>IF((B155=""),"",VLOOKUP(B155,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Environmental Assessment Certificate GRANTED</v>
-      </c>
-      <c r="D155" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="E155" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="F155" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G155" s="2">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7">
-      <c r="A156" s="2">
-        <v>155</v>
-      </c>
-      <c r="B156" s="3">
-        <v>64</v>
-      </c>
-      <c r="C156" s="4" t="str">
-        <f>IF((B156=""),"",VLOOKUP(B156,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Environmental Assessment Certificate GRANTED</v>
-      </c>
-      <c r="D156" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E156" s="30" t="s">
-        <v>197</v>
-      </c>
-      <c r="F156" s="1" t="s">
-        <v>337</v>
-      </c>
-      <c r="G156" s="2">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7">
-      <c r="A157" s="2">
-        <v>156</v>
-      </c>
-      <c r="B157" s="3">
-        <v>65</v>
-      </c>
-      <c r="C157" s="4" t="str">
-        <f>IF((B157=""),"",VLOOKUP(B157,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Environmental Assessment Certificate REFUSED</v>
-      </c>
-      <c r="D157" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="E157" s="9" t="s">
-        <v>195</v>
-      </c>
-      <c r="F157" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="G157" s="2">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7">
-      <c r="A158" s="2">
-        <v>157</v>
-      </c>
-      <c r="B158" s="3">
-        <v>65</v>
-      </c>
-      <c r="C158" s="4" t="str">
-        <f>IF((B158=""),"",VLOOKUP(B158,[1]Outcomes!$A$2:$D$66,4,FALSE))</f>
-        <v>Environmental Assessment Certificate REFUSED</v>
-      </c>
-      <c r="D158" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="E158" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="F158" s="1" t="s">
-        <v>328</v>
-      </c>
-      <c r="G158" s="2">
-        <v>157</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G158" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
+  <autoFilter ref="A1:G137" xr:uid="{00000000-0001-0000-0400-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
@@ -26720,13 +26153,13 @@
           <x14:formula1>
             <xm:f>Lookups!$U$3:$U$16</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D58 D63:D81 D90 D95 D104 D109 D115 D120 D129 D134 D143 D148 D154</xm:sqref>
+          <xm:sqref>D2:D50 D55:D71</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Outcomes!$A$2:$A$30</xm:f>
           </x14:formula1>
-          <xm:sqref>B2:B81</xm:sqref>
+          <xm:sqref>B2:B71</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -28406,17 +27839,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2C1F259FB5F1743B0AABDE6E19F3587" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="887a673b2990ad08cbc7da39ce2412c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9da97c54-3012-49fd-8896-0db67528b2a3" xmlns:ns3="a10d9883-6879-4486-9776-c67b50dca88e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e318ef65ff943bae84f18b0edea6bb11" ns2:_="" ns3:_="">
     <xsd:import namespace="9da97c54-3012-49fd-8896-0db67528b2a3"/>
@@ -28645,6 +28067,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="9da97c54-3012-49fd-8896-0db67528b2a3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="a10d9883-6879-4486-9776-c67b50dca88e" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -28655,17 +28088,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
-    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{21ADD561-5989-478E-9183-7F2CBAD25CE1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -28684,6 +28106,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1383CF79-2DB2-40C6-9ED2-5A25DF7BC797}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="9da97c54-3012-49fd-8896-0db67528b2a3"/>
+    <ds:schemaRef ds:uri="a10d9883-6879-4486-9776-c67b50dca88e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C7D293B7-B48B-419C-B420-25F67C616F6F}">
   <ds:schemaRefs>

</xml_diff>